<commit_message>
Updated documentation and the region map file
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5d5170efd4f85cb/Documents/Model Railroading/NMRAMembers/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="425" documentId="14_{7CC62D34-1848-8E45-94BC-59B517219C12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81277A27-A579-7140-89D9-32E8149D99D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F2D6E-E11E-6343-A769-7959268D68A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-74120" yWindow="1040" windowWidth="29520" windowHeight="40520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="111360" yWindow="14040" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division Reassignments" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="215">
   <si>
     <t>division</t>
   </si>
@@ -672,9 +672,6 @@
   </si>
   <si>
     <t>TLR</t>
-  </si>
-  <si>
-    <t>Former Lakeshores</t>
   </si>
   <si>
     <t>Unknown</t>
@@ -684,7 +681,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1103,13 +1100,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
@@ -1117,7 +1114,7 @@
     <col min="4" max="4" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1147,7 +1144,7 @@
         <v>000</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>21</v>
       </c>
@@ -1161,7 +1158,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>21</v>
       </c>
@@ -1175,7 +1172,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1189,7 +1186,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>21</v>
       </c>
@@ -1203,7 +1200,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>21</v>
       </c>
@@ -1217,7 +1214,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>21</v>
       </c>
@@ -1231,7 +1228,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>21</v>
       </c>
@@ -1245,7 +1242,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>21</v>
       </c>
@@ -1259,7 +1256,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>21</v>
       </c>
@@ -1273,7 +1270,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>21</v>
       </c>
@@ -1287,7 +1284,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>21</v>
       </c>
@@ -1301,7 +1298,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>21</v>
       </c>
@@ -1315,7 +1312,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>21</v>
       </c>
@@ -1329,7 +1326,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>21</v>
       </c>
@@ -1343,12 +1340,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
@@ -1357,7 +1354,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>22</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>22</v>
       </c>
@@ -1385,7 +1382,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>22</v>
       </c>
@@ -1399,2516 +1396,2502 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>214</v>
+        <v>120</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>23</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>23</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>23</v>
       </c>
       <c r="B31" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>23</v>
       </c>
       <c r="B32" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>23</v>
       </c>
       <c r="B33" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>23</v>
       </c>
       <c r="B34" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>23</v>
       </c>
       <c r="B35" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>24</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>24</v>
       </c>
       <c r="B38" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>24</v>
       </c>
       <c r="B39" s="1">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>24</v>
       </c>
       <c r="B40" s="1">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>24</v>
       </c>
       <c r="B41" s="1">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>24</v>
       </c>
       <c r="B42" s="1">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>24</v>
       </c>
       <c r="B43" s="1">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44" s="1">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>25</v>
       </c>
       <c r="B45" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>25</v>
       </c>
       <c r="B46" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>25</v>
       </c>
       <c r="B47" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>25</v>
       </c>
       <c r="B48" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>25</v>
       </c>
       <c r="B49" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>25</v>
       </c>
       <c r="B50" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>25</v>
       </c>
       <c r="B51" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B52" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>26</v>
       </c>
       <c r="B53" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>26</v>
       </c>
       <c r="B54" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>26</v>
       </c>
       <c r="B55" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>26</v>
       </c>
       <c r="B56" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>26</v>
       </c>
       <c r="B57" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B58" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>27</v>
       </c>
       <c r="B59" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>27</v>
       </c>
       <c r="B60" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>27</v>
       </c>
       <c r="B61" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>27</v>
       </c>
       <c r="B62" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>27</v>
       </c>
       <c r="B63" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>27</v>
       </c>
       <c r="B64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>27</v>
       </c>
       <c r="B65" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>27</v>
       </c>
       <c r="B66" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>27</v>
       </c>
       <c r="B67" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>27</v>
       </c>
       <c r="B68" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>27</v>
       </c>
       <c r="B69" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>27</v>
       </c>
       <c r="B70" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>27</v>
       </c>
       <c r="B71" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>27</v>
       </c>
       <c r="B72" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>27</v>
       </c>
       <c r="B73" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>27</v>
       </c>
       <c r="B74" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>27</v>
       </c>
       <c r="B75" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B76" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>28</v>
       </c>
       <c r="B77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>28</v>
       </c>
       <c r="B78" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>28</v>
       </c>
       <c r="B79" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>28</v>
       </c>
       <c r="B80" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>28</v>
       </c>
       <c r="B81" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>28</v>
       </c>
       <c r="B82" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>28</v>
       </c>
       <c r="B83" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>28</v>
       </c>
       <c r="B84" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>28</v>
       </c>
       <c r="B85" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>28</v>
       </c>
       <c r="B86" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B87" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>29</v>
       </c>
       <c r="B88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>29</v>
       </c>
       <c r="B89" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>29</v>
       </c>
       <c r="B90" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>29</v>
       </c>
       <c r="B91" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>29</v>
       </c>
       <c r="B92" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>29</v>
       </c>
       <c r="B93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>29</v>
       </c>
       <c r="B94" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>29</v>
       </c>
       <c r="B95" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>29</v>
       </c>
       <c r="B96" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>29</v>
       </c>
       <c r="B97" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>29</v>
       </c>
       <c r="B98" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>29</v>
       </c>
       <c r="B99" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>29</v>
       </c>
       <c r="B100" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>29</v>
       </c>
       <c r="B101" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>29</v>
       </c>
       <c r="B102" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>29</v>
       </c>
       <c r="B103" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>29</v>
       </c>
       <c r="B104" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>29</v>
       </c>
       <c r="B105" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>29</v>
       </c>
       <c r="B106" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>29</v>
       </c>
       <c r="B107" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>29</v>
       </c>
       <c r="B108" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>29</v>
       </c>
       <c r="B109" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B110" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>30</v>
       </c>
       <c r="B111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>30</v>
       </c>
       <c r="B112" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>30</v>
       </c>
       <c r="B113" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>30</v>
       </c>
       <c r="B114" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>30</v>
       </c>
       <c r="B115" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>30</v>
       </c>
       <c r="B116" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>30</v>
       </c>
       <c r="B118" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>30</v>
       </c>
       <c r="B119" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>30</v>
       </c>
       <c r="B120" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>30</v>
       </c>
       <c r="B121" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>30</v>
       </c>
       <c r="B123" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B124" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>31</v>
       </c>
       <c r="B125" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>31</v>
       </c>
       <c r="B126" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>31</v>
       </c>
       <c r="B127" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>31</v>
       </c>
       <c r="B128" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>31</v>
       </c>
       <c r="B129" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>31</v>
       </c>
       <c r="B130" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>31</v>
       </c>
       <c r="B131" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>31</v>
       </c>
       <c r="B132" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B133" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>32</v>
       </c>
       <c r="B134" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>32</v>
       </c>
       <c r="B135" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>32</v>
       </c>
       <c r="B136" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>32</v>
       </c>
       <c r="B137" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>32</v>
       </c>
       <c r="B138" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>32</v>
       </c>
       <c r="B139" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>32</v>
       </c>
       <c r="B140" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>32</v>
       </c>
       <c r="B141" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>32</v>
       </c>
       <c r="B142" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>32</v>
       </c>
       <c r="B143" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>32</v>
       </c>
       <c r="B144" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B145" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>64</v>
+        <v>168</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>33</v>
       </c>
       <c r="B146" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>33</v>
       </c>
       <c r="B147" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>33</v>
       </c>
       <c r="B148" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>33</v>
       </c>
       <c r="B149" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>33</v>
       </c>
       <c r="B150" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>33</v>
       </c>
       <c r="B151" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>33</v>
       </c>
       <c r="B152" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B163" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>170</v>
+        <v>29</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>34</v>
       </c>
       <c r="B164" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>34</v>
       </c>
       <c r="B165" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>34</v>
       </c>
       <c r="B166" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>34</v>
       </c>
       <c r="B167" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>34</v>
       </c>
       <c r="B168" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>34</v>
       </c>
       <c r="B169" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>34</v>
       </c>
       <c r="B170" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B177" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>36</v>
       </c>
       <c r="B178" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>36</v>
       </c>
       <c r="B179" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>36</v>
       </c>
       <c r="B180" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>35</v>
+        <v>186</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>36</v>
       </c>
       <c r="B181" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B182" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>37</v>
       </c>
       <c r="B183" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>37</v>
       </c>
       <c r="B184" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>37</v>
       </c>
       <c r="B185" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>37</v>
       </c>
       <c r="B186" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B187" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>147</v>
+        <v>18</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>38</v>
       </c>
       <c r="B188" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>38</v>
       </c>
       <c r="B189" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>38</v>
       </c>
       <c r="B190" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>38</v>
       </c>
       <c r="B191" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>38</v>
       </c>
       <c r="B192" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>38</v>
       </c>
       <c r="B193" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>38</v>
       </c>
       <c r="B194" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>38</v>
       </c>
       <c r="B195" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B198" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4">
-      <c r="A199" s="1">
-        <v>39</v>
-      </c>
-      <c r="B199" s="1">
-        <v>0</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D199" s="2" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D199">
-    <sortCondition ref="A3:A199"/>
-    <sortCondition ref="B3:B199"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D198">
+    <sortCondition ref="A3:A198"/>
+    <sortCondition ref="B3:B198"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added entry for new NER Lakeshores Division per NMRA website
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F2D6E-E11E-6343-A769-7959268D68A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD118A-DF6E-BA46-92E3-F85B5BFD9F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="111360" yWindow="14040" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="215">
   <si>
     <t>division</t>
   </si>
@@ -1100,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1342,10 +1342,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
@@ -1359,13 +1359,13 @@
         <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1373,10 +1373,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>204</v>
@@ -1387,10 +1387,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>204</v>
@@ -1401,10 +1401,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>204</v>
@@ -1415,10 +1415,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>204</v>
@@ -1429,10 +1429,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>204</v>
@@ -1443,10 +1443,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>204</v>
@@ -1457,10 +1457,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>204</v>
@@ -1468,16 +1468,16 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1485,10 +1485,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>205</v>
@@ -1499,10 +1499,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>205</v>
@@ -1513,10 +1513,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>205</v>
@@ -1527,10 +1527,10 @@
         <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>205</v>
@@ -1541,10 +1541,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>205</v>
@@ -1555,10 +1555,10 @@
         <v>23</v>
       </c>
       <c r="B32" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>205</v>
@@ -1569,10 +1569,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>205</v>
@@ -1583,10 +1583,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>205</v>
@@ -1597,10 +1597,10 @@
         <v>23</v>
       </c>
       <c r="B35" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>205</v>
@@ -1608,16 +1608,16 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1625,10 +1625,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>213</v>
@@ -1639,10 +1639,10 @@
         <v>24</v>
       </c>
       <c r="B38" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>213</v>
@@ -1653,10 +1653,10 @@
         <v>24</v>
       </c>
       <c r="B39" s="1">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>213</v>
@@ -1667,10 +1667,10 @@
         <v>24</v>
       </c>
       <c r="B40" s="1">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>213</v>
@@ -1681,10 +1681,10 @@
         <v>24</v>
       </c>
       <c r="B41" s="1">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>213</v>
@@ -1695,10 +1695,10 @@
         <v>24</v>
       </c>
       <c r="B42" s="1">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>213</v>
@@ -1709,10 +1709,10 @@
         <v>24</v>
       </c>
       <c r="B43" s="1">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>213</v>
@@ -1720,16 +1720,16 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1737,10 +1737,10 @@
         <v>25</v>
       </c>
       <c r="B45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>208</v>
@@ -1751,10 +1751,10 @@
         <v>25</v>
       </c>
       <c r="B46" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>208</v>
@@ -1765,10 +1765,10 @@
         <v>25</v>
       </c>
       <c r="B47" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>208</v>
@@ -1779,10 +1779,10 @@
         <v>25</v>
       </c>
       <c r="B48" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>208</v>
@@ -1793,10 +1793,10 @@
         <v>25</v>
       </c>
       <c r="B49" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>208</v>
@@ -1807,10 +1807,10 @@
         <v>25</v>
       </c>
       <c r="B50" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>208</v>
@@ -1821,10 +1821,10 @@
         <v>25</v>
       </c>
       <c r="B51" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>208</v>
@@ -1832,16 +1832,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,10 +1849,10 @@
         <v>26</v>
       </c>
       <c r="B53" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>207</v>
@@ -1863,10 +1863,10 @@
         <v>26</v>
       </c>
       <c r="B54" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>207</v>
@@ -1877,10 +1877,10 @@
         <v>26</v>
       </c>
       <c r="B55" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>207</v>
@@ -1891,10 +1891,10 @@
         <v>26</v>
       </c>
       <c r="B56" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>207</v>
@@ -1905,10 +1905,10 @@
         <v>26</v>
       </c>
       <c r="B57" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>207</v>
@@ -1916,16 +1916,16 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B58" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1933,10 +1933,10 @@
         <v>27</v>
       </c>
       <c r="B59" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>210</v>
@@ -1947,10 +1947,10 @@
         <v>27</v>
       </c>
       <c r="B60" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>210</v>
@@ -1961,10 +1961,10 @@
         <v>27</v>
       </c>
       <c r="B61" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>210</v>
@@ -1975,10 +1975,10 @@
         <v>27</v>
       </c>
       <c r="B62" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>210</v>
@@ -1989,10 +1989,10 @@
         <v>27</v>
       </c>
       <c r="B63" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>210</v>
@@ -2003,10 +2003,10 @@
         <v>27</v>
       </c>
       <c r="B64" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>210</v>
@@ -2017,10 +2017,10 @@
         <v>27</v>
       </c>
       <c r="B65" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>210</v>
@@ -2031,10 +2031,10 @@
         <v>27</v>
       </c>
       <c r="B66" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>210</v>
@@ -2045,10 +2045,10 @@
         <v>27</v>
       </c>
       <c r="B67" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>210</v>
@@ -2059,10 +2059,10 @@
         <v>27</v>
       </c>
       <c r="B68" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>210</v>
@@ -2073,10 +2073,10 @@
         <v>27</v>
       </c>
       <c r="B69" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>210</v>
@@ -2087,10 +2087,10 @@
         <v>27</v>
       </c>
       <c r="B70" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>210</v>
@@ -2101,10 +2101,10 @@
         <v>27</v>
       </c>
       <c r="B71" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>210</v>
@@ -2115,10 +2115,10 @@
         <v>27</v>
       </c>
       <c r="B72" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>210</v>
@@ -2129,10 +2129,10 @@
         <v>27</v>
       </c>
       <c r="B73" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>210</v>
@@ -2143,10 +2143,10 @@
         <v>27</v>
       </c>
       <c r="B74" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>210</v>
@@ -2157,10 +2157,10 @@
         <v>27</v>
       </c>
       <c r="B75" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>210</v>
@@ -2168,16 +2168,16 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B76" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2185,10 +2185,10 @@
         <v>28</v>
       </c>
       <c r="B77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>203</v>
@@ -2199,10 +2199,10 @@
         <v>28</v>
       </c>
       <c r="B78" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>203</v>
@@ -2213,10 +2213,10 @@
         <v>28</v>
       </c>
       <c r="B79" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>203</v>
@@ -2227,10 +2227,10 @@
         <v>28</v>
       </c>
       <c r="B80" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>203</v>
@@ -2241,10 +2241,10 @@
         <v>28</v>
       </c>
       <c r="B81" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>203</v>
@@ -2255,10 +2255,10 @@
         <v>28</v>
       </c>
       <c r="B82" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>203</v>
@@ -2269,10 +2269,10 @@
         <v>28</v>
       </c>
       <c r="B83" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>203</v>
@@ -2283,10 +2283,10 @@
         <v>28</v>
       </c>
       <c r="B84" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>203</v>
@@ -2297,10 +2297,10 @@
         <v>28</v>
       </c>
       <c r="B85" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>203</v>
@@ -2311,10 +2311,10 @@
         <v>28</v>
       </c>
       <c r="B86" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>203</v>
@@ -2322,16 +2322,16 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B87" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2339,10 +2339,10 @@
         <v>29</v>
       </c>
       <c r="B88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>201</v>
@@ -2353,10 +2353,10 @@
         <v>29</v>
       </c>
       <c r="B89" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>201</v>
@@ -2367,10 +2367,10 @@
         <v>29</v>
       </c>
       <c r="B90" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>201</v>
@@ -2381,10 +2381,10 @@
         <v>29</v>
       </c>
       <c r="B91" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>201</v>
@@ -2395,10 +2395,10 @@
         <v>29</v>
       </c>
       <c r="B92" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>201</v>
@@ -2409,10 +2409,10 @@
         <v>29</v>
       </c>
       <c r="B93" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>201</v>
@@ -2423,10 +2423,10 @@
         <v>29</v>
       </c>
       <c r="B94" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>201</v>
@@ -2437,10 +2437,10 @@
         <v>29</v>
       </c>
       <c r="B95" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>201</v>
@@ -2451,10 +2451,10 @@
         <v>29</v>
       </c>
       <c r="B96" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>201</v>
@@ -2465,10 +2465,10 @@
         <v>29</v>
       </c>
       <c r="B97" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>201</v>
@@ -2479,10 +2479,10 @@
         <v>29</v>
       </c>
       <c r="B98" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>201</v>
@@ -2493,10 +2493,10 @@
         <v>29</v>
       </c>
       <c r="B99" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>201</v>
@@ -2507,10 +2507,10 @@
         <v>29</v>
       </c>
       <c r="B100" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>201</v>
@@ -2521,10 +2521,10 @@
         <v>29</v>
       </c>
       <c r="B101" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>201</v>
@@ -2535,10 +2535,10 @@
         <v>29</v>
       </c>
       <c r="B102" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>201</v>
@@ -2549,10 +2549,10 @@
         <v>29</v>
       </c>
       <c r="B103" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>201</v>
@@ -2563,10 +2563,10 @@
         <v>29</v>
       </c>
       <c r="B104" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>201</v>
@@ -2577,10 +2577,10 @@
         <v>29</v>
       </c>
       <c r="B105" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>201</v>
@@ -2591,10 +2591,10 @@
         <v>29</v>
       </c>
       <c r="B106" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>201</v>
@@ -2605,10 +2605,10 @@
         <v>29</v>
       </c>
       <c r="B107" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>201</v>
@@ -2619,10 +2619,10 @@
         <v>29</v>
       </c>
       <c r="B108" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>201</v>
@@ -2633,10 +2633,10 @@
         <v>29</v>
       </c>
       <c r="B109" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>201</v>
@@ -2644,16 +2644,16 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B110" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2661,10 +2661,10 @@
         <v>30</v>
       </c>
       <c r="B111" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>202</v>
@@ -2675,10 +2675,10 @@
         <v>30</v>
       </c>
       <c r="B112" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>202</v>
@@ -2689,10 +2689,10 @@
         <v>30</v>
       </c>
       <c r="B113" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>202</v>
@@ -2703,10 +2703,10 @@
         <v>30</v>
       </c>
       <c r="B114" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>202</v>
@@ -2717,10 +2717,10 @@
         <v>30</v>
       </c>
       <c r="B115" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>202</v>
@@ -2731,10 +2731,10 @@
         <v>30</v>
       </c>
       <c r="B116" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>202</v>
@@ -2745,10 +2745,10 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>202</v>
@@ -2759,10 +2759,10 @@
         <v>30</v>
       </c>
       <c r="B118" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>202</v>
@@ -2773,10 +2773,10 @@
         <v>30</v>
       </c>
       <c r="B119" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>202</v>
@@ -2787,10 +2787,10 @@
         <v>30</v>
       </c>
       <c r="B120" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>202</v>
@@ -2801,10 +2801,10 @@
         <v>30</v>
       </c>
       <c r="B121" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>202</v>
@@ -2815,10 +2815,10 @@
         <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>202</v>
@@ -2829,10 +2829,10 @@
         <v>30</v>
       </c>
       <c r="B123" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>202</v>
@@ -2840,16 +2840,16 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B124" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2857,10 +2857,10 @@
         <v>31</v>
       </c>
       <c r="B125" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>199</v>
@@ -2871,10 +2871,10 @@
         <v>31</v>
       </c>
       <c r="B126" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>199</v>
@@ -2885,10 +2885,10 @@
         <v>31</v>
       </c>
       <c r="B127" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>199</v>
@@ -2899,10 +2899,10 @@
         <v>31</v>
       </c>
       <c r="B128" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>199</v>
@@ -2913,10 +2913,10 @@
         <v>31</v>
       </c>
       <c r="B129" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>199</v>
@@ -2927,10 +2927,10 @@
         <v>31</v>
       </c>
       <c r="B130" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>199</v>
@@ -2941,10 +2941,10 @@
         <v>31</v>
       </c>
       <c r="B131" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>199</v>
@@ -2955,10 +2955,10 @@
         <v>31</v>
       </c>
       <c r="B132" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>199</v>
@@ -2966,16 +2966,16 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B133" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2983,10 +2983,10 @@
         <v>32</v>
       </c>
       <c r="B134" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>200</v>
@@ -2997,10 +2997,10 @@
         <v>32</v>
       </c>
       <c r="B135" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>200</v>
@@ -3011,10 +3011,10 @@
         <v>32</v>
       </c>
       <c r="B136" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>200</v>
@@ -3025,10 +3025,10 @@
         <v>32</v>
       </c>
       <c r="B137" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>200</v>
@@ -3039,10 +3039,10 @@
         <v>32</v>
       </c>
       <c r="B138" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>200</v>
@@ -3053,10 +3053,10 @@
         <v>32</v>
       </c>
       <c r="B139" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>200</v>
@@ -3067,10 +3067,10 @@
         <v>32</v>
       </c>
       <c r="B140" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>200</v>
@@ -3081,10 +3081,10 @@
         <v>32</v>
       </c>
       <c r="B141" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>200</v>
@@ -3095,10 +3095,10 @@
         <v>32</v>
       </c>
       <c r="B142" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>200</v>
@@ -3109,10 +3109,10 @@
         <v>32</v>
       </c>
       <c r="B143" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>200</v>
@@ -3123,10 +3123,10 @@
         <v>32</v>
       </c>
       <c r="B144" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>200</v>
@@ -3134,16 +3134,16 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B145" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -3151,10 +3151,10 @@
         <v>33</v>
       </c>
       <c r="B146" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>211</v>
@@ -3165,10 +3165,10 @@
         <v>33</v>
       </c>
       <c r="B147" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>211</v>
@@ -3179,10 +3179,10 @@
         <v>33</v>
       </c>
       <c r="B148" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>211</v>
@@ -3193,10 +3193,10 @@
         <v>33</v>
       </c>
       <c r="B149" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>211</v>
@@ -3207,10 +3207,10 @@
         <v>33</v>
       </c>
       <c r="B150" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>211</v>
@@ -3221,10 +3221,10 @@
         <v>33</v>
       </c>
       <c r="B151" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>211</v>
@@ -3235,10 +3235,10 @@
         <v>33</v>
       </c>
       <c r="B152" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>211</v>
@@ -3249,10 +3249,10 @@
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>211</v>
@@ -3263,10 +3263,10 @@
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>211</v>
@@ -3277,10 +3277,10 @@
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>211</v>
@@ -3291,10 +3291,10 @@
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>211</v>
@@ -3305,10 +3305,10 @@
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>211</v>
@@ -3319,10 +3319,10 @@
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>211</v>
@@ -3333,10 +3333,10 @@
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>211</v>
@@ -3347,10 +3347,10 @@
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>211</v>
@@ -3361,10 +3361,10 @@
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>211</v>
@@ -3375,10 +3375,10 @@
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>211</v>
@@ -3386,16 +3386,16 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B163" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3403,10 +3403,10 @@
         <v>34</v>
       </c>
       <c r="B164" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>197</v>
@@ -3417,10 +3417,10 @@
         <v>34</v>
       </c>
       <c r="B165" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>197</v>
@@ -3431,10 +3431,10 @@
         <v>34</v>
       </c>
       <c r="B166" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>197</v>
@@ -3445,10 +3445,10 @@
         <v>34</v>
       </c>
       <c r="B167" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>197</v>
@@ -3459,10 +3459,10 @@
         <v>34</v>
       </c>
       <c r="B168" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>197</v>
@@ -3473,10 +3473,10 @@
         <v>34</v>
       </c>
       <c r="B169" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>197</v>
@@ -3487,10 +3487,10 @@
         <v>34</v>
       </c>
       <c r="B170" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>197</v>
@@ -3501,10 +3501,10 @@
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>197</v>
@@ -3515,10 +3515,10 @@
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>197</v>
@@ -3529,10 +3529,10 @@
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>197</v>
@@ -3543,10 +3543,10 @@
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>197</v>
@@ -3557,10 +3557,10 @@
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>197</v>
@@ -3571,10 +3571,10 @@
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>197</v>
@@ -3582,16 +3582,16 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B177" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>184</v>
+        <v>42</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -3599,10 +3599,10 @@
         <v>36</v>
       </c>
       <c r="B178" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>212</v>
@@ -3613,10 +3613,10 @@
         <v>36</v>
       </c>
       <c r="B179" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>212</v>
@@ -3627,10 +3627,10 @@
         <v>36</v>
       </c>
       <c r="B180" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>212</v>
@@ -3641,10 +3641,10 @@
         <v>36</v>
       </c>
       <c r="B181" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>212</v>
@@ -3652,16 +3652,16 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B182" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -3669,10 +3669,10 @@
         <v>37</v>
       </c>
       <c r="B183" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>209</v>
@@ -3683,10 +3683,10 @@
         <v>37</v>
       </c>
       <c r="B184" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>209</v>
@@ -3697,10 +3697,10 @@
         <v>37</v>
       </c>
       <c r="B185" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>209</v>
@@ -3711,10 +3711,10 @@
         <v>37</v>
       </c>
       <c r="B186" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>209</v>
@@ -3722,16 +3722,16 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B187" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -3739,10 +3739,10 @@
         <v>38</v>
       </c>
       <c r="B188" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>196</v>
@@ -3753,10 +3753,10 @@
         <v>38</v>
       </c>
       <c r="B189" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>196</v>
@@ -3767,10 +3767,10 @@
         <v>38</v>
       </c>
       <c r="B190" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>196</v>
@@ -3781,10 +3781,10 @@
         <v>38</v>
       </c>
       <c r="B191" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>196</v>
@@ -3795,10 +3795,10 @@
         <v>38</v>
       </c>
       <c r="B192" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>196</v>
@@ -3809,10 +3809,10 @@
         <v>38</v>
       </c>
       <c r="B193" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>196</v>
@@ -3823,10 +3823,10 @@
         <v>38</v>
       </c>
       <c r="B194" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>196</v>
@@ -3837,10 +3837,10 @@
         <v>38</v>
       </c>
       <c r="B195" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>196</v>
@@ -3851,10 +3851,10 @@
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>196</v>
@@ -3865,10 +3865,10 @@
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>196</v>
@@ -3876,22 +3876,36 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
+        <v>38</v>
+      </c>
+      <c r="B198" s="1">
+        <v>10</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
         <v>39</v>
       </c>
-      <c r="B198" s="1">
+      <c r="B199" s="1">
         <v>0</v>
       </c>
-      <c r="C198" s="2" t="s">
+      <c r="C199" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D198" s="2" t="s">
+      <c r="D199" s="2" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D198">
-    <sortCondition ref="A3:A198"/>
-    <sortCondition ref="B3:B198"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D199">
+    <sortCondition ref="A3:A199"/>
+    <sortCondition ref="B3:B199"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fixes for zip file generation
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD118A-DF6E-BA46-92E3-F85B5BFD9F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45ABDDB-4EE8-E548-B068-862934231010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="111360" yWindow="14040" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division Reassignments" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="215">
   <si>
     <t>division</t>
   </si>
@@ -1100,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2465,10 +2465,10 @@
         <v>29</v>
       </c>
       <c r="B97" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>201</v>
@@ -2479,10 +2479,10 @@
         <v>29</v>
       </c>
       <c r="B98" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>201</v>
@@ -2493,10 +2493,10 @@
         <v>29</v>
       </c>
       <c r="B99" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>201</v>
@@ -2507,10 +2507,10 @@
         <v>29</v>
       </c>
       <c r="B100" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>201</v>
@@ -2521,10 +2521,10 @@
         <v>29</v>
       </c>
       <c r="B101" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>201</v>
@@ -2535,10 +2535,10 @@
         <v>29</v>
       </c>
       <c r="B102" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>201</v>
@@ -2549,10 +2549,10 @@
         <v>29</v>
       </c>
       <c r="B103" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>201</v>
@@ -2563,10 +2563,10 @@
         <v>29</v>
       </c>
       <c r="B104" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>201</v>
@@ -2577,10 +2577,10 @@
         <v>29</v>
       </c>
       <c r="B105" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>201</v>
@@ -2591,10 +2591,10 @@
         <v>29</v>
       </c>
       <c r="B106" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>201</v>
@@ -2605,10 +2605,10 @@
         <v>29</v>
       </c>
       <c r="B107" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>201</v>
@@ -2619,10 +2619,10 @@
         <v>29</v>
       </c>
       <c r="B108" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>201</v>
@@ -2633,10 +2633,10 @@
         <v>29</v>
       </c>
       <c r="B109" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>201</v>
@@ -2647,10 +2647,10 @@
         <v>29</v>
       </c>
       <c r="B110" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>201</v>
@@ -2658,16 +2658,16 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B111" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2675,10 +2675,10 @@
         <v>30</v>
       </c>
       <c r="B112" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>202</v>
@@ -2689,10 +2689,10 @@
         <v>30</v>
       </c>
       <c r="B113" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>202</v>
@@ -2703,10 +2703,10 @@
         <v>30</v>
       </c>
       <c r="B114" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>202</v>
@@ -2717,10 +2717,10 @@
         <v>30</v>
       </c>
       <c r="B115" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>202</v>
@@ -2731,10 +2731,10 @@
         <v>30</v>
       </c>
       <c r="B116" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>202</v>
@@ -2745,10 +2745,10 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>202</v>
@@ -2759,10 +2759,10 @@
         <v>30</v>
       </c>
       <c r="B118" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>202</v>
@@ -2773,10 +2773,10 @@
         <v>30</v>
       </c>
       <c r="B119" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>202</v>
@@ -2787,10 +2787,10 @@
         <v>30</v>
       </c>
       <c r="B120" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>202</v>
@@ -2801,10 +2801,10 @@
         <v>30</v>
       </c>
       <c r="B121" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>202</v>
@@ -2815,10 +2815,10 @@
         <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>202</v>
@@ -2829,10 +2829,10 @@
         <v>30</v>
       </c>
       <c r="B123" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>202</v>
@@ -2843,10 +2843,10 @@
         <v>30</v>
       </c>
       <c r="B124" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>202</v>
@@ -2854,16 +2854,16 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B125" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2871,10 +2871,10 @@
         <v>31</v>
       </c>
       <c r="B126" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>199</v>
@@ -2885,10 +2885,10 @@
         <v>31</v>
       </c>
       <c r="B127" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>199</v>
@@ -2899,10 +2899,10 @@
         <v>31</v>
       </c>
       <c r="B128" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>199</v>
@@ -2913,10 +2913,10 @@
         <v>31</v>
       </c>
       <c r="B129" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>199</v>
@@ -2927,10 +2927,10 @@
         <v>31</v>
       </c>
       <c r="B130" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>199</v>
@@ -2941,10 +2941,10 @@
         <v>31</v>
       </c>
       <c r="B131" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>199</v>
@@ -2955,10 +2955,10 @@
         <v>31</v>
       </c>
       <c r="B132" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>199</v>
@@ -2969,10 +2969,10 @@
         <v>31</v>
       </c>
       <c r="B133" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>199</v>
@@ -2980,16 +2980,16 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B134" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -2997,10 +2997,10 @@
         <v>32</v>
       </c>
       <c r="B135" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>200</v>
@@ -3011,10 +3011,10 @@
         <v>32</v>
       </c>
       <c r="B136" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>200</v>
@@ -3025,10 +3025,10 @@
         <v>32</v>
       </c>
       <c r="B137" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>200</v>
@@ -3039,10 +3039,10 @@
         <v>32</v>
       </c>
       <c r="B138" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>200</v>
@@ -3053,10 +3053,10 @@
         <v>32</v>
       </c>
       <c r="B139" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>200</v>
@@ -3067,10 +3067,10 @@
         <v>32</v>
       </c>
       <c r="B140" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>200</v>
@@ -3081,10 +3081,10 @@
         <v>32</v>
       </c>
       <c r="B141" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>200</v>
@@ -3095,10 +3095,10 @@
         <v>32</v>
       </c>
       <c r="B142" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>200</v>
@@ -3109,10 +3109,10 @@
         <v>32</v>
       </c>
       <c r="B143" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>200</v>
@@ -3123,10 +3123,10 @@
         <v>32</v>
       </c>
       <c r="B144" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>200</v>
@@ -3137,10 +3137,10 @@
         <v>32</v>
       </c>
       <c r="B145" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>200</v>
@@ -3148,16 +3148,16 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B146" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -3165,10 +3165,10 @@
         <v>33</v>
       </c>
       <c r="B147" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>211</v>
@@ -3179,10 +3179,10 @@
         <v>33</v>
       </c>
       <c r="B148" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>211</v>
@@ -3193,10 +3193,10 @@
         <v>33</v>
       </c>
       <c r="B149" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>211</v>
@@ -3207,10 +3207,10 @@
         <v>33</v>
       </c>
       <c r="B150" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>211</v>
@@ -3221,10 +3221,10 @@
         <v>33</v>
       </c>
       <c r="B151" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>211</v>
@@ -3235,10 +3235,10 @@
         <v>33</v>
       </c>
       <c r="B152" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>211</v>
@@ -3249,10 +3249,10 @@
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>211</v>
@@ -3263,10 +3263,10 @@
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>211</v>
@@ -3277,10 +3277,10 @@
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>211</v>
@@ -3291,10 +3291,10 @@
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>211</v>
@@ -3305,10 +3305,10 @@
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>211</v>
@@ -3319,10 +3319,10 @@
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>211</v>
@@ -3333,10 +3333,10 @@
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>211</v>
@@ -3347,10 +3347,10 @@
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>211</v>
@@ -3361,10 +3361,10 @@
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>211</v>
@@ -3375,10 +3375,10 @@
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>211</v>
@@ -3389,10 +3389,10 @@
         <v>33</v>
       </c>
       <c r="B163" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>211</v>
@@ -3400,16 +3400,16 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B164" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3417,10 +3417,10 @@
         <v>34</v>
       </c>
       <c r="B165" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>197</v>
@@ -3431,10 +3431,10 @@
         <v>34</v>
       </c>
       <c r="B166" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>197</v>
@@ -3445,10 +3445,10 @@
         <v>34</v>
       </c>
       <c r="B167" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>197</v>
@@ -3459,10 +3459,10 @@
         <v>34</v>
       </c>
       <c r="B168" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>197</v>
@@ -3473,10 +3473,10 @@
         <v>34</v>
       </c>
       <c r="B169" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>197</v>
@@ -3487,10 +3487,10 @@
         <v>34</v>
       </c>
       <c r="B170" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>197</v>
@@ -3501,10 +3501,10 @@
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>197</v>
@@ -3515,10 +3515,10 @@
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>197</v>
@@ -3529,10 +3529,10 @@
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>197</v>
@@ -3543,10 +3543,10 @@
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>197</v>
@@ -3557,10 +3557,10 @@
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>197</v>
@@ -3571,10 +3571,10 @@
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>197</v>
@@ -3585,10 +3585,10 @@
         <v>34</v>
       </c>
       <c r="B177" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>197</v>
@@ -3596,16 +3596,16 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B178" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>184</v>
+        <v>42</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -3613,10 +3613,10 @@
         <v>36</v>
       </c>
       <c r="B179" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>212</v>
@@ -3627,10 +3627,10 @@
         <v>36</v>
       </c>
       <c r="B180" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>212</v>
@@ -3641,10 +3641,10 @@
         <v>36</v>
       </c>
       <c r="B181" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>212</v>
@@ -3655,10 +3655,10 @@
         <v>36</v>
       </c>
       <c r="B182" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>212</v>
@@ -3666,16 +3666,16 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B183" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -3683,10 +3683,10 @@
         <v>37</v>
       </c>
       <c r="B184" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>209</v>
@@ -3697,10 +3697,10 @@
         <v>37</v>
       </c>
       <c r="B185" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>209</v>
@@ -3711,10 +3711,10 @@
         <v>37</v>
       </c>
       <c r="B186" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>209</v>
@@ -3725,10 +3725,10 @@
         <v>37</v>
       </c>
       <c r="B187" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>209</v>
@@ -3736,16 +3736,16 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B188" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -3753,10 +3753,10 @@
         <v>38</v>
       </c>
       <c r="B189" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>196</v>
@@ -3767,10 +3767,10 @@
         <v>38</v>
       </c>
       <c r="B190" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>196</v>
@@ -3781,10 +3781,10 @@
         <v>38</v>
       </c>
       <c r="B191" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>196</v>
@@ -3795,10 +3795,10 @@
         <v>38</v>
       </c>
       <c r="B192" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>196</v>
@@ -3809,10 +3809,10 @@
         <v>38</v>
       </c>
       <c r="B193" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>196</v>
@@ -3823,10 +3823,10 @@
         <v>38</v>
       </c>
       <c r="B194" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>196</v>
@@ -3837,10 +3837,10 @@
         <v>38</v>
       </c>
       <c r="B195" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>196</v>
@@ -3851,10 +3851,10 @@
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>196</v>
@@ -3865,10 +3865,10 @@
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>196</v>
@@ -3879,10 +3879,10 @@
         <v>38</v>
       </c>
       <c r="B198" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>196</v>
@@ -3890,22 +3890,36 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
+        <v>38</v>
+      </c>
+      <c r="B199" s="1">
+        <v>10</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
         <v>39</v>
       </c>
-      <c r="B199" s="1">
+      <c r="B200" s="1">
         <v>0</v>
       </c>
-      <c r="C199" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D199" s="2" t="s">
+      <c r="D200" s="2" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D199">
-    <sortCondition ref="A3:A199"/>
-    <sortCondition ref="B3:B199"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D200">
+    <sortCondition ref="A3:A200"/>
+    <sortCondition ref="B3:B200"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bugs in zip file generation
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45ABDDB-4EE8-E548-B068-862934231010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21044E0D-3874-6048-8F91-5320667079C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="215">
   <si>
     <t>division</t>
   </si>
@@ -1100,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D200"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1356,13 +1356,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>206</v>
@@ -1373,13 +1373,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1387,10 +1387,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>204</v>
@@ -1401,10 +1401,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>204</v>
@@ -1415,10 +1415,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>204</v>
@@ -1429,10 +1429,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>204</v>
@@ -1443,10 +1443,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>204</v>
@@ -1457,10 +1457,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>204</v>
@@ -1471,10 +1471,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>204</v>
@@ -1482,16 +1482,16 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1499,10 +1499,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>205</v>
@@ -1513,10 +1513,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>205</v>
@@ -1527,10 +1527,10 @@
         <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>205</v>
@@ -1541,10 +1541,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>205</v>
@@ -1555,10 +1555,10 @@
         <v>23</v>
       </c>
       <c r="B32" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>205</v>
@@ -1569,10 +1569,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>205</v>
@@ -1583,10 +1583,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>205</v>
@@ -1597,10 +1597,10 @@
         <v>23</v>
       </c>
       <c r="B35" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>205</v>
@@ -1611,10 +1611,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>205</v>
@@ -1622,16 +1622,16 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1639,10 +1639,10 @@
         <v>24</v>
       </c>
       <c r="B38" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>213</v>
@@ -1653,10 +1653,10 @@
         <v>24</v>
       </c>
       <c r="B39" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>213</v>
@@ -1667,10 +1667,10 @@
         <v>24</v>
       </c>
       <c r="B40" s="1">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>213</v>
@@ -1681,10 +1681,10 @@
         <v>24</v>
       </c>
       <c r="B41" s="1">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>213</v>
@@ -1695,10 +1695,10 @@
         <v>24</v>
       </c>
       <c r="B42" s="1">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>213</v>
@@ -1709,10 +1709,10 @@
         <v>24</v>
       </c>
       <c r="B43" s="1">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>213</v>
@@ -1723,10 +1723,10 @@
         <v>24</v>
       </c>
       <c r="B44" s="1">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>213</v>
@@ -1734,16 +1734,16 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45" s="1">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1751,10 +1751,10 @@
         <v>25</v>
       </c>
       <c r="B46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>208</v>
@@ -1765,10 +1765,10 @@
         <v>25</v>
       </c>
       <c r="B47" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>208</v>
@@ -1779,10 +1779,10 @@
         <v>25</v>
       </c>
       <c r="B48" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>208</v>
@@ -1793,10 +1793,10 @@
         <v>25</v>
       </c>
       <c r="B49" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>208</v>
@@ -1807,10 +1807,10 @@
         <v>25</v>
       </c>
       <c r="B50" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>208</v>
@@ -1821,10 +1821,10 @@
         <v>25</v>
       </c>
       <c r="B51" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>208</v>
@@ -1835,10 +1835,10 @@
         <v>25</v>
       </c>
       <c r="B52" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>208</v>
@@ -1846,16 +1846,16 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1863,10 +1863,10 @@
         <v>26</v>
       </c>
       <c r="B54" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>207</v>
@@ -1877,10 +1877,10 @@
         <v>26</v>
       </c>
       <c r="B55" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>207</v>
@@ -1891,10 +1891,10 @@
         <v>26</v>
       </c>
       <c r="B56" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>207</v>
@@ -1905,10 +1905,10 @@
         <v>26</v>
       </c>
       <c r="B57" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>207</v>
@@ -1919,10 +1919,10 @@
         <v>26</v>
       </c>
       <c r="B58" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>207</v>
@@ -1930,16 +1930,16 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1947,10 +1947,10 @@
         <v>27</v>
       </c>
       <c r="B60" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>210</v>
@@ -1961,10 +1961,10 @@
         <v>27</v>
       </c>
       <c r="B61" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>210</v>
@@ -1975,10 +1975,10 @@
         <v>27</v>
       </c>
       <c r="B62" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>210</v>
@@ -1989,10 +1989,10 @@
         <v>27</v>
       </c>
       <c r="B63" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>210</v>
@@ -2003,10 +2003,10 @@
         <v>27</v>
       </c>
       <c r="B64" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>210</v>
@@ -2017,10 +2017,10 @@
         <v>27</v>
       </c>
       <c r="B65" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>210</v>
@@ -2031,10 +2031,10 @@
         <v>27</v>
       </c>
       <c r="B66" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>210</v>
@@ -2045,10 +2045,10 @@
         <v>27</v>
       </c>
       <c r="B67" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>210</v>
@@ -2059,10 +2059,10 @@
         <v>27</v>
       </c>
       <c r="B68" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>210</v>
@@ -2073,10 +2073,10 @@
         <v>27</v>
       </c>
       <c r="B69" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>210</v>
@@ -2087,10 +2087,10 @@
         <v>27</v>
       </c>
       <c r="B70" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>210</v>
@@ -2101,10 +2101,10 @@
         <v>27</v>
       </c>
       <c r="B71" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>210</v>
@@ -2115,10 +2115,10 @@
         <v>27</v>
       </c>
       <c r="B72" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>210</v>
@@ -2129,10 +2129,10 @@
         <v>27</v>
       </c>
       <c r="B73" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>210</v>
@@ -2143,10 +2143,10 @@
         <v>27</v>
       </c>
       <c r="B74" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>210</v>
@@ -2157,10 +2157,10 @@
         <v>27</v>
       </c>
       <c r="B75" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>210</v>
@@ -2171,10 +2171,10 @@
         <v>27</v>
       </c>
       <c r="B76" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>210</v>
@@ -2182,16 +2182,16 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B77" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2199,10 +2199,10 @@
         <v>28</v>
       </c>
       <c r="B78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>203</v>
@@ -2213,10 +2213,10 @@
         <v>28</v>
       </c>
       <c r="B79" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>203</v>
@@ -2227,10 +2227,10 @@
         <v>28</v>
       </c>
       <c r="B80" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>203</v>
@@ -2241,10 +2241,10 @@
         <v>28</v>
       </c>
       <c r="B81" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>203</v>
@@ -2255,10 +2255,10 @@
         <v>28</v>
       </c>
       <c r="B82" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>203</v>
@@ -2269,10 +2269,10 @@
         <v>28</v>
       </c>
       <c r="B83" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>203</v>
@@ -2283,10 +2283,10 @@
         <v>28</v>
       </c>
       <c r="B84" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>203</v>
@@ -2297,10 +2297,10 @@
         <v>28</v>
       </c>
       <c r="B85" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>203</v>
@@ -2311,10 +2311,10 @@
         <v>28</v>
       </c>
       <c r="B86" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>203</v>
@@ -2325,10 +2325,10 @@
         <v>28</v>
       </c>
       <c r="B87" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>203</v>
@@ -2336,16 +2336,16 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B88" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2353,10 +2353,10 @@
         <v>29</v>
       </c>
       <c r="B89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>201</v>
@@ -2367,10 +2367,10 @@
         <v>29</v>
       </c>
       <c r="B90" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>201</v>
@@ -2381,10 +2381,10 @@
         <v>29</v>
       </c>
       <c r="B91" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>201</v>
@@ -2395,10 +2395,10 @@
         <v>29</v>
       </c>
       <c r="B92" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>201</v>
@@ -2409,10 +2409,10 @@
         <v>29</v>
       </c>
       <c r="B93" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>201</v>
@@ -2423,10 +2423,10 @@
         <v>29</v>
       </c>
       <c r="B94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>201</v>
@@ -2437,10 +2437,10 @@
         <v>29</v>
       </c>
       <c r="B95" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>201</v>
@@ -2451,10 +2451,10 @@
         <v>29</v>
       </c>
       <c r="B96" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>201</v>
@@ -2465,10 +2465,10 @@
         <v>29</v>
       </c>
       <c r="B97" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>201</v>
@@ -2479,10 +2479,10 @@
         <v>29</v>
       </c>
       <c r="B98" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>201</v>
@@ -2493,10 +2493,10 @@
         <v>29</v>
       </c>
       <c r="B99" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>201</v>
@@ -2507,10 +2507,10 @@
         <v>29</v>
       </c>
       <c r="B100" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>201</v>
@@ -2521,10 +2521,10 @@
         <v>29</v>
       </c>
       <c r="B101" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>201</v>
@@ -2535,10 +2535,10 @@
         <v>29</v>
       </c>
       <c r="B102" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>201</v>
@@ -2549,10 +2549,10 @@
         <v>29</v>
       </c>
       <c r="B103" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>201</v>
@@ -2563,10 +2563,10 @@
         <v>29</v>
       </c>
       <c r="B104" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>201</v>
@@ -2577,10 +2577,10 @@
         <v>29</v>
       </c>
       <c r="B105" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>201</v>
@@ -2591,10 +2591,10 @@
         <v>29</v>
       </c>
       <c r="B106" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>201</v>
@@ -2605,10 +2605,10 @@
         <v>29</v>
       </c>
       <c r="B107" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>201</v>
@@ -2619,10 +2619,10 @@
         <v>29</v>
       </c>
       <c r="B108" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>201</v>
@@ -2633,10 +2633,10 @@
         <v>29</v>
       </c>
       <c r="B109" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>201</v>
@@ -2647,10 +2647,10 @@
         <v>29</v>
       </c>
       <c r="B110" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>201</v>
@@ -2661,10 +2661,10 @@
         <v>29</v>
       </c>
       <c r="B111" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>201</v>
@@ -2672,16 +2672,16 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B112" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2689,10 +2689,10 @@
         <v>30</v>
       </c>
       <c r="B113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>202</v>
@@ -2703,10 +2703,10 @@
         <v>30</v>
       </c>
       <c r="B114" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>202</v>
@@ -2717,10 +2717,10 @@
         <v>30</v>
       </c>
       <c r="B115" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>202</v>
@@ -2731,10 +2731,10 @@
         <v>30</v>
       </c>
       <c r="B116" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>202</v>
@@ -2745,10 +2745,10 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>202</v>
@@ -2759,10 +2759,10 @@
         <v>30</v>
       </c>
       <c r="B118" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>202</v>
@@ -2773,10 +2773,10 @@
         <v>30</v>
       </c>
       <c r="B119" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>202</v>
@@ -2787,10 +2787,10 @@
         <v>30</v>
       </c>
       <c r="B120" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>202</v>
@@ -2801,10 +2801,10 @@
         <v>30</v>
       </c>
       <c r="B121" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>202</v>
@@ -2815,10 +2815,10 @@
         <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>202</v>
@@ -2829,10 +2829,10 @@
         <v>30</v>
       </c>
       <c r="B123" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>202</v>
@@ -2843,10 +2843,10 @@
         <v>30</v>
       </c>
       <c r="B124" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>202</v>
@@ -2857,10 +2857,10 @@
         <v>30</v>
       </c>
       <c r="B125" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>202</v>
@@ -2868,16 +2868,16 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B126" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2885,10 +2885,10 @@
         <v>31</v>
       </c>
       <c r="B127" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>199</v>
@@ -2899,10 +2899,10 @@
         <v>31</v>
       </c>
       <c r="B128" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>199</v>
@@ -2913,10 +2913,10 @@
         <v>31</v>
       </c>
       <c r="B129" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>199</v>
@@ -2927,10 +2927,10 @@
         <v>31</v>
       </c>
       <c r="B130" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>199</v>
@@ -2941,10 +2941,10 @@
         <v>31</v>
       </c>
       <c r="B131" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>199</v>
@@ -2955,10 +2955,10 @@
         <v>31</v>
       </c>
       <c r="B132" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>199</v>
@@ -2969,10 +2969,10 @@
         <v>31</v>
       </c>
       <c r="B133" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>199</v>
@@ -2983,10 +2983,10 @@
         <v>31</v>
       </c>
       <c r="B134" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>199</v>
@@ -2994,16 +2994,16 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B135" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -3011,10 +3011,10 @@
         <v>32</v>
       </c>
       <c r="B136" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>200</v>
@@ -3025,10 +3025,10 @@
         <v>32</v>
       </c>
       <c r="B137" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>200</v>
@@ -3039,10 +3039,10 @@
         <v>32</v>
       </c>
       <c r="B138" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>200</v>
@@ -3053,10 +3053,10 @@
         <v>32</v>
       </c>
       <c r="B139" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>200</v>
@@ -3067,10 +3067,10 @@
         <v>32</v>
       </c>
       <c r="B140" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>200</v>
@@ -3081,10 +3081,10 @@
         <v>32</v>
       </c>
       <c r="B141" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>200</v>
@@ -3095,10 +3095,10 @@
         <v>32</v>
       </c>
       <c r="B142" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>200</v>
@@ -3109,10 +3109,10 @@
         <v>32</v>
       </c>
       <c r="B143" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>200</v>
@@ -3123,10 +3123,10 @@
         <v>32</v>
       </c>
       <c r="B144" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>200</v>
@@ -3137,10 +3137,10 @@
         <v>32</v>
       </c>
       <c r="B145" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>200</v>
@@ -3151,10 +3151,10 @@
         <v>32</v>
       </c>
       <c r="B146" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>200</v>
@@ -3162,16 +3162,16 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B147" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -3179,10 +3179,10 @@
         <v>33</v>
       </c>
       <c r="B148" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>211</v>
@@ -3193,10 +3193,10 @@
         <v>33</v>
       </c>
       <c r="B149" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>211</v>
@@ -3207,10 +3207,10 @@
         <v>33</v>
       </c>
       <c r="B150" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>211</v>
@@ -3221,10 +3221,10 @@
         <v>33</v>
       </c>
       <c r="B151" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>211</v>
@@ -3235,10 +3235,10 @@
         <v>33</v>
       </c>
       <c r="B152" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>211</v>
@@ -3249,10 +3249,10 @@
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>211</v>
@@ -3263,10 +3263,10 @@
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>211</v>
@@ -3277,10 +3277,10 @@
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>211</v>
@@ -3291,10 +3291,10 @@
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>211</v>
@@ -3305,10 +3305,10 @@
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>211</v>
@@ -3319,10 +3319,10 @@
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>211</v>
@@ -3333,10 +3333,10 @@
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>211</v>
@@ -3347,10 +3347,10 @@
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>211</v>
@@ -3361,10 +3361,10 @@
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>211</v>
@@ -3375,10 +3375,10 @@
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>211</v>
@@ -3389,10 +3389,10 @@
         <v>33</v>
       </c>
       <c r="B163" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>211</v>
@@ -3403,10 +3403,10 @@
         <v>33</v>
       </c>
       <c r="B164" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>211</v>
@@ -3414,16 +3414,16 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B165" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3431,10 +3431,10 @@
         <v>34</v>
       </c>
       <c r="B166" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>197</v>
@@ -3445,10 +3445,10 @@
         <v>34</v>
       </c>
       <c r="B167" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>197</v>
@@ -3459,10 +3459,10 @@
         <v>34</v>
       </c>
       <c r="B168" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>197</v>
@@ -3473,10 +3473,10 @@
         <v>34</v>
       </c>
       <c r="B169" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>197</v>
@@ -3487,10 +3487,10 @@
         <v>34</v>
       </c>
       <c r="B170" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>197</v>
@@ -3501,10 +3501,10 @@
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>197</v>
@@ -3515,10 +3515,10 @@
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>197</v>
@@ -3529,10 +3529,10 @@
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>197</v>
@@ -3543,10 +3543,10 @@
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>197</v>
@@ -3557,10 +3557,10 @@
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>197</v>
@@ -3571,10 +3571,10 @@
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>197</v>
@@ -3585,10 +3585,10 @@
         <v>34</v>
       </c>
       <c r="B177" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>197</v>
@@ -3599,10 +3599,10 @@
         <v>34</v>
       </c>
       <c r="B178" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>197</v>
@@ -3610,16 +3610,16 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B179" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>184</v>
+        <v>42</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -3627,10 +3627,10 @@
         <v>36</v>
       </c>
       <c r="B180" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>212</v>
@@ -3641,10 +3641,10 @@
         <v>36</v>
       </c>
       <c r="B181" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>212</v>
@@ -3655,10 +3655,10 @@
         <v>36</v>
       </c>
       <c r="B182" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>212</v>
@@ -3669,10 +3669,10 @@
         <v>36</v>
       </c>
       <c r="B183" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>212</v>
@@ -3680,16 +3680,16 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B184" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -3697,10 +3697,10 @@
         <v>37</v>
       </c>
       <c r="B185" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>209</v>
@@ -3711,10 +3711,10 @@
         <v>37</v>
       </c>
       <c r="B186" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>209</v>
@@ -3725,10 +3725,10 @@
         <v>37</v>
       </c>
       <c r="B187" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>209</v>
@@ -3739,10 +3739,10 @@
         <v>37</v>
       </c>
       <c r="B188" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>209</v>
@@ -3750,16 +3750,16 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B189" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -3767,10 +3767,10 @@
         <v>38</v>
       </c>
       <c r="B190" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>196</v>
@@ -3781,10 +3781,10 @@
         <v>38</v>
       </c>
       <c r="B191" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>196</v>
@@ -3795,10 +3795,10 @@
         <v>38</v>
       </c>
       <c r="B192" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>196</v>
@@ -3809,10 +3809,10 @@
         <v>38</v>
       </c>
       <c r="B193" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>196</v>
@@ -3823,10 +3823,10 @@
         <v>38</v>
       </c>
       <c r="B194" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>196</v>
@@ -3837,10 +3837,10 @@
         <v>38</v>
       </c>
       <c r="B195" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>196</v>
@@ -3851,10 +3851,10 @@
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>196</v>
@@ -3865,10 +3865,10 @@
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>196</v>
@@ -3879,10 +3879,10 @@
         <v>38</v>
       </c>
       <c r="B198" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>196</v>
@@ -3893,10 +3893,10 @@
         <v>38</v>
       </c>
       <c r="B199" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>196</v>
@@ -3904,22 +3904,36 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
+        <v>38</v>
+      </c>
+      <c r="B200" s="1">
+        <v>10</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
         <v>39</v>
       </c>
-      <c r="B200" s="1">
+      <c r="B201" s="1">
         <v>0</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="C201" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D200" s="2" t="s">
+      <c r="D201" s="2" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D200">
-    <sortCondition ref="A3:A200"/>
-    <sortCondition ref="B3:B200"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D201">
+    <sortCondition ref="A3:A201"/>
+    <sortCondition ref="B3:B201"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support for Apple M1 silicon
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21044E0D-3874-6048-8F91-5320667079C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2AC65F-D20D-5648-B479-D210D560A16B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37780" yWindow="15760" windowWidth="39020" windowHeight="27440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division Reassignments" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="216">
   <si>
     <t>division</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Allegheny Western Division</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3176,16 +3179,16 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B148" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -3193,10 +3196,10 @@
         <v>33</v>
       </c>
       <c r="B149" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>211</v>
@@ -3207,10 +3210,10 @@
         <v>33</v>
       </c>
       <c r="B150" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>211</v>
@@ -3221,10 +3224,10 @@
         <v>33</v>
       </c>
       <c r="B151" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>211</v>
@@ -3235,10 +3238,10 @@
         <v>33</v>
       </c>
       <c r="B152" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>211</v>
@@ -3249,10 +3252,10 @@
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>211</v>
@@ -3263,10 +3266,10 @@
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>211</v>
@@ -3277,10 +3280,10 @@
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>211</v>
@@ -3291,10 +3294,10 @@
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>211</v>
@@ -3305,10 +3308,10 @@
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>211</v>
@@ -3319,10 +3322,10 @@
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>211</v>
@@ -3333,10 +3336,10 @@
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>211</v>
@@ -3347,10 +3350,10 @@
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>211</v>
@@ -3361,10 +3364,10 @@
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>211</v>
@@ -3375,10 +3378,10 @@
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>211</v>
@@ -3389,10 +3392,10 @@
         <v>33</v>
       </c>
       <c r="B163" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>211</v>
@@ -3403,10 +3406,10 @@
         <v>33</v>
       </c>
       <c r="B164" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>211</v>
@@ -3417,10 +3420,10 @@
         <v>33</v>
       </c>
       <c r="B165" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>211</v>
@@ -3428,16 +3431,16 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B166" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3445,10 +3448,10 @@
         <v>34</v>
       </c>
       <c r="B167" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>197</v>
@@ -3459,10 +3462,10 @@
         <v>34</v>
       </c>
       <c r="B168" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>197</v>
@@ -3473,10 +3476,10 @@
         <v>34</v>
       </c>
       <c r="B169" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>197</v>
@@ -3487,10 +3490,10 @@
         <v>34</v>
       </c>
       <c r="B170" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>197</v>
@@ -3501,10 +3504,10 @@
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>197</v>
@@ -3515,10 +3518,10 @@
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>197</v>
@@ -3529,10 +3532,10 @@
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>197</v>
@@ -3543,10 +3546,10 @@
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>197</v>
@@ -3557,10 +3560,10 @@
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>197</v>
@@ -3571,10 +3574,10 @@
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>197</v>
@@ -3585,10 +3588,10 @@
         <v>34</v>
       </c>
       <c r="B177" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>197</v>
@@ -3599,10 +3602,10 @@
         <v>34</v>
       </c>
       <c r="B178" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>197</v>
@@ -3613,10 +3616,10 @@
         <v>34</v>
       </c>
       <c r="B179" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>197</v>
@@ -3624,16 +3627,16 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B180" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>184</v>
+        <v>42</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -3641,10 +3644,10 @@
         <v>36</v>
       </c>
       <c r="B181" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>212</v>
@@ -3655,10 +3658,10 @@
         <v>36</v>
       </c>
       <c r="B182" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>212</v>
@@ -3669,10 +3672,10 @@
         <v>36</v>
       </c>
       <c r="B183" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>212</v>
@@ -3683,10 +3686,10 @@
         <v>36</v>
       </c>
       <c r="B184" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>212</v>
@@ -3694,16 +3697,16 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B185" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -3711,10 +3714,10 @@
         <v>37</v>
       </c>
       <c r="B186" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>209</v>
@@ -3725,10 +3728,10 @@
         <v>37</v>
       </c>
       <c r="B187" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>209</v>
@@ -3739,10 +3742,10 @@
         <v>37</v>
       </c>
       <c r="B188" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>209</v>
@@ -3753,10 +3756,10 @@
         <v>37</v>
       </c>
       <c r="B189" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>209</v>
@@ -3764,16 +3767,16 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B190" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -3781,10 +3784,10 @@
         <v>38</v>
       </c>
       <c r="B191" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>196</v>
@@ -3795,10 +3798,10 @@
         <v>38</v>
       </c>
       <c r="B192" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>196</v>
@@ -3809,10 +3812,10 @@
         <v>38</v>
       </c>
       <c r="B193" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>196</v>
@@ -3823,10 +3826,10 @@
         <v>38</v>
       </c>
       <c r="B194" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>196</v>
@@ -3837,10 +3840,10 @@
         <v>38</v>
       </c>
       <c r="B195" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>196</v>
@@ -3851,10 +3854,10 @@
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>196</v>
@@ -3865,10 +3868,10 @@
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>196</v>
@@ -3879,10 +3882,10 @@
         <v>38</v>
       </c>
       <c r="B198" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>196</v>
@@ -3893,10 +3896,10 @@
         <v>38</v>
       </c>
       <c r="B199" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>196</v>
@@ -3907,10 +3910,10 @@
         <v>38</v>
       </c>
       <c r="B200" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>196</v>
@@ -3918,22 +3921,36 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
+        <v>38</v>
+      </c>
+      <c r="B201" s="1">
+        <v>10</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
         <v>39</v>
       </c>
-      <c r="B201" s="1">
+      <c r="B202" s="1">
         <v>0</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="C202" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D201" s="2" t="s">
+      <c r="D202" s="2" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D201">
-    <sortCondition ref="A3:A201"/>
-    <sortCondition ref="B3:B201"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D202">
+    <sortCondition ref="A3:A202"/>
+    <sortCondition ref="B3:B202"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to latest NMRA Map
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2AC65F-D20D-5648-B479-D210D560A16B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B83CCF-FF21-BA4F-A696-AB220CC66A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37780" yWindow="15760" windowWidth="39020" windowHeight="27440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division Reassignments" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="218">
   <si>
     <t>division</t>
   </si>
@@ -678,6 +678,12 @@
   </si>
   <si>
     <t>Allegheny Western Division</t>
+  </si>
+  <si>
+    <t>NEW BR DIVISION</t>
+  </si>
+  <si>
+    <t>Division 7</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D202"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1600,10 +1606,10 @@
         <v>23</v>
       </c>
       <c r="B35" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>128</v>
+        <v>217</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>205</v>
@@ -1614,10 +1620,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>205</v>
@@ -1628,10 +1634,10 @@
         <v>23</v>
       </c>
       <c r="B37" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>205</v>
@@ -1639,16 +1645,16 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1656,10 +1662,10 @@
         <v>24</v>
       </c>
       <c r="B39" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>213</v>
@@ -1670,10 +1676,10 @@
         <v>24</v>
       </c>
       <c r="B40" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>213</v>
@@ -1684,10 +1690,10 @@
         <v>24</v>
       </c>
       <c r="B41" s="1">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>213</v>
@@ -1698,10 +1704,10 @@
         <v>24</v>
       </c>
       <c r="B42" s="1">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>213</v>
@@ -1712,10 +1718,10 @@
         <v>24</v>
       </c>
       <c r="B43" s="1">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>213</v>
@@ -1726,10 +1732,10 @@
         <v>24</v>
       </c>
       <c r="B44" s="1">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>213</v>
@@ -1740,10 +1746,10 @@
         <v>24</v>
       </c>
       <c r="B45" s="1">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>168</v>
+        <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>213</v>
@@ -1751,30 +1757,30 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>137</v>
+        <v>192</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" s="1">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1782,10 +1788,10 @@
         <v>25</v>
       </c>
       <c r="B48" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>208</v>
@@ -1796,10 +1802,10 @@
         <v>25</v>
       </c>
       <c r="B49" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>208</v>
@@ -1810,10 +1816,10 @@
         <v>25</v>
       </c>
       <c r="B50" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>208</v>
@@ -1824,10 +1830,10 @@
         <v>25</v>
       </c>
       <c r="B51" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>208</v>
@@ -1838,10 +1844,10 @@
         <v>25</v>
       </c>
       <c r="B52" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>208</v>
@@ -1852,10 +1858,10 @@
         <v>25</v>
       </c>
       <c r="B53" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>208</v>
@@ -1863,30 +1869,30 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B54" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1894,10 +1900,10 @@
         <v>26</v>
       </c>
       <c r="B56" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>207</v>
@@ -1908,10 +1914,10 @@
         <v>26</v>
       </c>
       <c r="B57" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>207</v>
@@ -1922,10 +1928,10 @@
         <v>26</v>
       </c>
       <c r="B58" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>207</v>
@@ -1936,10 +1942,10 @@
         <v>26</v>
       </c>
       <c r="B59" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>207</v>
@@ -1947,30 +1953,30 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B61" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1978,10 +1984,10 @@
         <v>27</v>
       </c>
       <c r="B62" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>210</v>
@@ -1992,10 +1998,10 @@
         <v>27</v>
       </c>
       <c r="B63" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>210</v>
@@ -2006,10 +2012,10 @@
         <v>27</v>
       </c>
       <c r="B64" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>210</v>
@@ -2020,10 +2026,10 @@
         <v>27</v>
       </c>
       <c r="B65" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>210</v>
@@ -2034,10 +2040,10 @@
         <v>27</v>
       </c>
       <c r="B66" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>210</v>
@@ -2048,10 +2054,10 @@
         <v>27</v>
       </c>
       <c r="B67" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>210</v>
@@ -2062,10 +2068,10 @@
         <v>27</v>
       </c>
       <c r="B68" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>210</v>
@@ -2076,10 +2082,10 @@
         <v>27</v>
       </c>
       <c r="B69" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>210</v>
@@ -2090,10 +2096,10 @@
         <v>27</v>
       </c>
       <c r="B70" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>210</v>
@@ -2104,10 +2110,10 @@
         <v>27</v>
       </c>
       <c r="B71" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>210</v>
@@ -2118,10 +2124,10 @@
         <v>27</v>
       </c>
       <c r="B72" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>210</v>
@@ -2132,10 +2138,10 @@
         <v>27</v>
       </c>
       <c r="B73" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>210</v>
@@ -2146,10 +2152,10 @@
         <v>27</v>
       </c>
       <c r="B74" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>210</v>
@@ -2160,10 +2166,10 @@
         <v>27</v>
       </c>
       <c r="B75" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>210</v>
@@ -2174,10 +2180,10 @@
         <v>27</v>
       </c>
       <c r="B76" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>210</v>
@@ -2188,10 +2194,10 @@
         <v>27</v>
       </c>
       <c r="B77" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>210</v>
@@ -2199,30 +2205,30 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B78" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B79" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2230,10 +2236,10 @@
         <v>28</v>
       </c>
       <c r="B80" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>203</v>
@@ -2244,10 +2250,10 @@
         <v>28</v>
       </c>
       <c r="B81" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>203</v>
@@ -2258,10 +2264,10 @@
         <v>28</v>
       </c>
       <c r="B82" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>203</v>
@@ -2272,10 +2278,10 @@
         <v>28</v>
       </c>
       <c r="B83" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>203</v>
@@ -2286,10 +2292,10 @@
         <v>28</v>
       </c>
       <c r="B84" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>203</v>
@@ -2300,10 +2306,10 @@
         <v>28</v>
       </c>
       <c r="B85" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>203</v>
@@ -2314,10 +2320,10 @@
         <v>28</v>
       </c>
       <c r="B86" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>203</v>
@@ -2328,10 +2334,10 @@
         <v>28</v>
       </c>
       <c r="B87" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>203</v>
@@ -2342,10 +2348,10 @@
         <v>28</v>
       </c>
       <c r="B88" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>203</v>
@@ -2353,30 +2359,30 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B89" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B90" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2384,10 +2390,10 @@
         <v>29</v>
       </c>
       <c r="B91" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>201</v>
@@ -2398,10 +2404,10 @@
         <v>29</v>
       </c>
       <c r="B92" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>201</v>
@@ -2412,10 +2418,10 @@
         <v>29</v>
       </c>
       <c r="B93" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>201</v>
@@ -2426,10 +2432,10 @@
         <v>29</v>
       </c>
       <c r="B94" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>201</v>
@@ -2440,10 +2446,10 @@
         <v>29</v>
       </c>
       <c r="B95" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>201</v>
@@ -2454,10 +2460,10 @@
         <v>29</v>
       </c>
       <c r="B96" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>201</v>
@@ -2468,10 +2474,10 @@
         <v>29</v>
       </c>
       <c r="B97" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>201</v>
@@ -2482,10 +2488,10 @@
         <v>29</v>
       </c>
       <c r="B98" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>201</v>
@@ -2496,10 +2502,10 @@
         <v>29</v>
       </c>
       <c r="B99" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>201</v>
@@ -2510,10 +2516,10 @@
         <v>29</v>
       </c>
       <c r="B100" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>201</v>
@@ -2524,10 +2530,10 @@
         <v>29</v>
       </c>
       <c r="B101" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>201</v>
@@ -2538,10 +2544,10 @@
         <v>29</v>
       </c>
       <c r="B102" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>201</v>
@@ -2552,10 +2558,10 @@
         <v>29</v>
       </c>
       <c r="B103" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>201</v>
@@ -2566,10 +2572,10 @@
         <v>29</v>
       </c>
       <c r="B104" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>201</v>
@@ -2580,10 +2586,10 @@
         <v>29</v>
       </c>
       <c r="B105" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>201</v>
@@ -2594,10 +2600,10 @@
         <v>29</v>
       </c>
       <c r="B106" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>201</v>
@@ -2608,10 +2614,10 @@
         <v>29</v>
       </c>
       <c r="B107" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>201</v>
@@ -2622,10 +2628,10 @@
         <v>29</v>
       </c>
       <c r="B108" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>201</v>
@@ -2636,10 +2642,10 @@
         <v>29</v>
       </c>
       <c r="B109" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>201</v>
@@ -2650,10 +2656,10 @@
         <v>29</v>
       </c>
       <c r="B110" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>201</v>
@@ -2664,10 +2670,10 @@
         <v>29</v>
       </c>
       <c r="B111" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>201</v>
@@ -2678,10 +2684,10 @@
         <v>29</v>
       </c>
       <c r="B112" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>201</v>
@@ -2689,30 +2695,30 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B113" s="1">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B114" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2720,10 +2726,10 @@
         <v>30</v>
       </c>
       <c r="B115" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>202</v>
@@ -2734,10 +2740,10 @@
         <v>30</v>
       </c>
       <c r="B116" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>202</v>
@@ -2748,10 +2754,10 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>202</v>
@@ -2762,10 +2768,10 @@
         <v>30</v>
       </c>
       <c r="B118" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>202</v>
@@ -2776,10 +2782,10 @@
         <v>30</v>
       </c>
       <c r="B119" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>202</v>
@@ -2790,10 +2796,10 @@
         <v>30</v>
       </c>
       <c r="B120" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>202</v>
@@ -2804,10 +2810,10 @@
         <v>30</v>
       </c>
       <c r="B121" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>202</v>
@@ -2818,10 +2824,10 @@
         <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>202</v>
@@ -2832,10 +2838,10 @@
         <v>30</v>
       </c>
       <c r="B123" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>202</v>
@@ -2846,10 +2852,10 @@
         <v>30</v>
       </c>
       <c r="B124" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>202</v>
@@ -2860,10 +2866,10 @@
         <v>30</v>
       </c>
       <c r="B125" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>202</v>
@@ -2874,10 +2880,10 @@
         <v>30</v>
       </c>
       <c r="B126" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>202</v>
@@ -2885,30 +2891,30 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B127" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B128" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -2916,10 +2922,10 @@
         <v>31</v>
       </c>
       <c r="B129" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>199</v>
@@ -2930,10 +2936,10 @@
         <v>31</v>
       </c>
       <c r="B130" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>199</v>
@@ -2944,10 +2950,10 @@
         <v>31</v>
       </c>
       <c r="B131" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>199</v>
@@ -2958,10 +2964,10 @@
         <v>31</v>
       </c>
       <c r="B132" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>199</v>
@@ -2972,10 +2978,10 @@
         <v>31</v>
       </c>
       <c r="B133" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>199</v>
@@ -2986,10 +2992,10 @@
         <v>31</v>
       </c>
       <c r="B134" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>199</v>
@@ -3000,10 +3006,10 @@
         <v>31</v>
       </c>
       <c r="B135" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>199</v>
@@ -3011,30 +3017,30 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B136" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B137" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -3042,10 +3048,10 @@
         <v>32</v>
       </c>
       <c r="B138" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>200</v>
@@ -3056,10 +3062,10 @@
         <v>32</v>
       </c>
       <c r="B139" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>200</v>
@@ -3070,10 +3076,10 @@
         <v>32</v>
       </c>
       <c r="B140" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>200</v>
@@ -3084,10 +3090,10 @@
         <v>32</v>
       </c>
       <c r="B141" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>200</v>
@@ -3098,10 +3104,10 @@
         <v>32</v>
       </c>
       <c r="B142" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>200</v>
@@ -3112,10 +3118,10 @@
         <v>32</v>
       </c>
       <c r="B143" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>200</v>
@@ -3126,10 +3132,10 @@
         <v>32</v>
       </c>
       <c r="B144" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>200</v>
@@ -3140,10 +3146,10 @@
         <v>32</v>
       </c>
       <c r="B145" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>200</v>
@@ -3154,10 +3160,10 @@
         <v>32</v>
       </c>
       <c r="B146" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>200</v>
@@ -3168,10 +3174,10 @@
         <v>32</v>
       </c>
       <c r="B147" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>200</v>
@@ -3182,10 +3188,10 @@
         <v>32</v>
       </c>
       <c r="B148" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>215</v>
+        <v>63</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>200</v>
@@ -3193,30 +3199,30 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B149" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B150" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>179</v>
+        <v>215</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -3224,10 +3230,10 @@
         <v>33</v>
       </c>
       <c r="B151" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>211</v>
@@ -3238,10 +3244,10 @@
         <v>33</v>
       </c>
       <c r="B152" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>211</v>
@@ -3252,10 +3258,10 @@
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>211</v>
@@ -3266,10 +3272,10 @@
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>95</v>
+        <v>175</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>211</v>
@@ -3280,10 +3286,10 @@
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>211</v>
@@ -3294,10 +3300,10 @@
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>211</v>
@@ -3308,10 +3314,10 @@
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>211</v>
@@ -3322,10 +3328,10 @@
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>211</v>
@@ -3336,10 +3342,10 @@
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>211</v>
@@ -3350,10 +3356,10 @@
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>211</v>
@@ -3364,10 +3370,10 @@
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>211</v>
@@ -3378,10 +3384,10 @@
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>211</v>
@@ -3392,10 +3398,10 @@
         <v>33</v>
       </c>
       <c r="B163" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>211</v>
@@ -3406,10 +3412,10 @@
         <v>33</v>
       </c>
       <c r="B164" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>211</v>
@@ -3420,10 +3426,10 @@
         <v>33</v>
       </c>
       <c r="B165" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>211</v>
@@ -3434,10 +3440,10 @@
         <v>33</v>
       </c>
       <c r="B166" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>211</v>
@@ -3445,30 +3451,30 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B167" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>29</v>
+        <v>181</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B168" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -3476,10 +3482,10 @@
         <v>34</v>
       </c>
       <c r="B169" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>197</v>
@@ -3490,10 +3496,10 @@
         <v>34</v>
       </c>
       <c r="B170" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>197</v>
@@ -3504,10 +3510,10 @@
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>197</v>
@@ -3518,10 +3524,10 @@
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>197</v>
@@ -3532,10 +3538,10 @@
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>197</v>
@@ -3546,10 +3552,10 @@
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>197</v>
@@ -3560,10 +3566,10 @@
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>197</v>
@@ -3574,10 +3580,10 @@
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>197</v>
@@ -3588,10 +3594,10 @@
         <v>34</v>
       </c>
       <c r="B177" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>197</v>
@@ -3602,10 +3608,10 @@
         <v>34</v>
       </c>
       <c r="B178" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>197</v>
@@ -3616,10 +3622,10 @@
         <v>34</v>
       </c>
       <c r="B179" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>197</v>
@@ -3630,10 +3636,10 @@
         <v>34</v>
       </c>
       <c r="B180" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>197</v>
@@ -3641,44 +3647,44 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B181" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>184</v>
+        <v>41</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B182" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>185</v>
+        <v>42</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B183" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>35</v>
+        <v>216</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -3686,10 +3692,10 @@
         <v>36</v>
       </c>
       <c r="B184" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>212</v>
@@ -3700,10 +3706,10 @@
         <v>36</v>
       </c>
       <c r="B185" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>212</v>
@@ -3711,44 +3717,44 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B186" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B187" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B188" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -3756,10 +3762,10 @@
         <v>37</v>
       </c>
       <c r="B189" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>209</v>
@@ -3770,10 +3776,10 @@
         <v>37</v>
       </c>
       <c r="B190" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>209</v>
@@ -3781,44 +3787,44 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B191" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B192" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B193" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -3826,10 +3832,10 @@
         <v>38</v>
       </c>
       <c r="B194" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>196</v>
@@ -3840,10 +3846,10 @@
         <v>38</v>
       </c>
       <c r="B195" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>196</v>
@@ -3854,10 +3860,10 @@
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>196</v>
@@ -3868,10 +3874,10 @@
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>196</v>
@@ -3882,10 +3888,10 @@
         <v>38</v>
       </c>
       <c r="B198" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>196</v>
@@ -3896,10 +3902,10 @@
         <v>38</v>
       </c>
       <c r="B199" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>196</v>
@@ -3910,10 +3916,10 @@
         <v>38</v>
       </c>
       <c r="B200" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>196</v>
@@ -3924,10 +3930,10 @@
         <v>38</v>
       </c>
       <c r="B201" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>196</v>
@@ -3935,22 +3941,64 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
+        <v>38</v>
+      </c>
+      <c r="B202" s="1">
+        <v>8</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>38</v>
+      </c>
+      <c r="B203" s="1">
+        <v>9</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>38</v>
+      </c>
+      <c r="B204" s="1">
+        <v>10</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
         <v>39</v>
       </c>
-      <c r="B202" s="1">
+      <c r="B205" s="1">
         <v>0</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="C205" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D202" s="2" t="s">
+      <c r="D205" s="2" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D202">
-    <sortCondition ref="A3:A202"/>
-    <sortCondition ref="B3:B202"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D205">
+    <sortCondition ref="A3:A205"/>
+    <sortCondition ref="B3:B205"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fixes with numerical formatting and added AppleScript for email distribution
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B83CCF-FF21-BA4F-A696-AB220CC66A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31FB1C9-AB21-5740-A24C-5CCD539F27E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37780" yWindow="15760" windowWidth="39020" windowHeight="27440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37820" yWindow="15760" windowWidth="38980" windowHeight="27440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Division Reassignments" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="221">
   <si>
     <t>division</t>
   </si>
@@ -371,9 +371,6 @@
     <t>Michiana</t>
   </si>
   <si>
-    <t>Niagra Frontier</t>
-  </si>
-  <si>
     <t>Allegheny Highlands</t>
   </si>
   <si>
@@ -684,6 +681,18 @@
   </si>
   <si>
     <t>Division 7</t>
+  </si>
+  <si>
+    <t>NMRA Unassigned</t>
+  </si>
+  <si>
+    <t>NFR Unassigned</t>
+  </si>
+  <si>
+    <t>NMRA</t>
+  </si>
+  <si>
+    <t>Southern Arkansas Area</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1144,13 +1153,11 @@
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="str">
-        <f>"00"</f>
-        <v>00</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f>"000"</f>
-        <v>000</v>
+      <c r="C2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1164,7 +1171,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1178,7 +1185,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1192,7 +1199,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1206,7 +1213,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1220,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1234,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1248,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1262,7 +1269,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1276,7 +1283,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1290,7 +1297,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1304,7 +1311,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1318,7 +1325,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1332,7 +1339,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1346,7 +1353,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1360,7 +1367,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1371,10 +1378,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1382,13 +1389,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1396,13 +1403,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,13 +1417,13 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1427,10 +1434,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1441,10 +1448,10 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1455,10 +1462,10 @@
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1469,10 +1476,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1483,10 +1490,10 @@
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1497,10 +1504,10 @@
         <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1511,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1525,10 +1532,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1539,10 +1546,10 @@
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1553,10 +1560,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1567,10 +1574,10 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1581,10 +1588,10 @@
         <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1595,10 +1602,10 @@
         <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1609,10 +1616,10 @@
         <v>7</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1623,10 +1630,10 @@
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1637,10 +1644,10 @@
         <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1651,10 +1658,10 @@
         <v>10</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1665,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1679,10 +1686,10 @@
         <v>10</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1693,10 +1700,10 @@
         <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1707,10 +1714,10 @@
         <v>51</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1721,10 +1728,10 @@
         <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1735,10 +1742,10 @@
         <v>62</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1752,7 +1759,7 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1763,10 +1770,10 @@
         <v>80</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1777,10 +1784,10 @@
         <v>91</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1791,10 +1798,10 @@
         <v>0</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1805,10 +1812,10 @@
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1819,10 +1826,10 @@
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1833,10 +1840,10 @@
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1847,10 +1854,10 @@
         <v>4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1861,10 +1868,10 @@
         <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1875,10 +1882,10 @@
         <v>6</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1889,10 +1896,10 @@
         <v>7</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1903,10 +1910,10 @@
         <v>0</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1917,10 +1924,10 @@
         <v>3</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1931,10 +1938,10 @@
         <v>4</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1945,10 +1952,10 @@
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1959,10 +1966,10 @@
         <v>7</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1973,10 +1980,10 @@
         <v>9</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1987,10 +1994,10 @@
         <v>0</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2001,10 +2008,10 @@
         <v>2</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2015,10 +2022,10 @@
         <v>3</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2029,10 +2036,10 @@
         <v>4</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2043,10 +2050,10 @@
         <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2057,10 +2064,10 @@
         <v>6</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2071,10 +2078,10 @@
         <v>7</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2085,10 +2092,10 @@
         <v>8</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2099,10 +2106,10 @@
         <v>9</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2113,10 +2120,10 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2127,10 +2134,10 @@
         <v>12</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2141,10 +2148,10 @@
         <v>13</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2155,10 +2162,10 @@
         <v>14</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2169,10 +2176,10 @@
         <v>15</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2183,10 +2190,10 @@
         <v>16</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2197,10 +2204,10 @@
         <v>17</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2211,10 +2218,10 @@
         <v>19</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2225,10 +2232,10 @@
         <v>20</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2242,7 +2249,7 @@
         <v>102</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2256,7 +2263,7 @@
         <v>103</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2270,7 +2277,7 @@
         <v>104</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2284,7 +2291,7 @@
         <v>105</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2298,7 +2305,7 @@
         <v>106</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2312,7 +2319,7 @@
         <v>107</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2326,7 +2333,7 @@
         <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2340,7 +2347,7 @@
         <v>109</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2354,7 +2361,7 @@
         <v>110</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2368,7 +2375,7 @@
         <v>111</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2382,7 +2389,7 @@
         <v>112</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2396,7 +2403,7 @@
         <v>65</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2410,7 +2417,7 @@
         <v>66</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2424,7 +2431,7 @@
         <v>67</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2438,7 +2445,7 @@
         <v>68</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2452,7 +2459,7 @@
         <v>69</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2466,7 +2473,7 @@
         <v>70</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2480,7 +2487,7 @@
         <v>71</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2494,7 +2501,7 @@
         <v>72</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2508,7 +2515,7 @@
         <v>73</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2522,7 +2529,7 @@
         <v>84</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2536,7 +2543,7 @@
         <v>74</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2550,7 +2557,7 @@
         <v>75</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2564,7 +2571,7 @@
         <v>76</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2578,7 +2585,7 @@
         <v>77</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2592,7 +2599,7 @@
         <v>78</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2606,7 +2613,7 @@
         <v>79</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2620,7 +2627,7 @@
         <v>80</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2634,7 +2641,7 @@
         <v>81</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2648,7 +2655,7 @@
         <v>82</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2662,7 +2669,7 @@
         <v>83</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2676,7 +2683,7 @@
         <v>84</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2690,7 +2697,7 @@
         <v>85</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2704,7 +2711,7 @@
         <v>86</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2718,21 +2725,21 @@
         <v>87</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B115" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>88</v>
+        <v>220</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2740,13 +2747,13 @@
         <v>30</v>
       </c>
       <c r="B116" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2754,13 +2761,13 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2768,13 +2775,13 @@
         <v>30</v>
       </c>
       <c r="B118" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2782,13 +2789,13 @@
         <v>30</v>
       </c>
       <c r="B119" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -2796,13 +2803,13 @@
         <v>30</v>
       </c>
       <c r="B120" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -2810,13 +2817,13 @@
         <v>30</v>
       </c>
       <c r="B121" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2824,13 +2831,13 @@
         <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2838,13 +2845,13 @@
         <v>30</v>
       </c>
       <c r="B123" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2852,13 +2859,13 @@
         <v>30</v>
       </c>
       <c r="B124" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2866,13 +2873,13 @@
         <v>30</v>
       </c>
       <c r="B125" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2880,13 +2887,13 @@
         <v>30</v>
       </c>
       <c r="B126" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2894,13 +2901,13 @@
         <v>30</v>
       </c>
       <c r="B127" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -2908,27 +2915,27 @@
         <v>30</v>
       </c>
       <c r="B128" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B129" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -2936,13 +2943,13 @@
         <v>31</v>
       </c>
       <c r="B130" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -2950,13 +2957,13 @@
         <v>31</v>
       </c>
       <c r="B131" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -2964,13 +2971,13 @@
         <v>31</v>
       </c>
       <c r="B132" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2978,13 +2985,13 @@
         <v>31</v>
       </c>
       <c r="B133" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2992,13 +2999,13 @@
         <v>31</v>
       </c>
       <c r="B134" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -3006,13 +3013,13 @@
         <v>31</v>
       </c>
       <c r="B135" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -3020,13 +3027,13 @@
         <v>31</v>
       </c>
       <c r="B136" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -3034,27 +3041,27 @@
         <v>31</v>
       </c>
       <c r="B137" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B138" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -3062,13 +3069,13 @@
         <v>32</v>
       </c>
       <c r="B139" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -3076,13 +3083,13 @@
         <v>32</v>
       </c>
       <c r="B140" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -3090,13 +3097,13 @@
         <v>32</v>
       </c>
       <c r="B141" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3104,13 +3111,13 @@
         <v>32</v>
       </c>
       <c r="B142" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -3118,13 +3125,13 @@
         <v>32</v>
       </c>
       <c r="B143" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3132,13 +3139,13 @@
         <v>32</v>
       </c>
       <c r="B144" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -3146,13 +3153,13 @@
         <v>32</v>
       </c>
       <c r="B145" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -3160,13 +3167,13 @@
         <v>32</v>
       </c>
       <c r="B146" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -3174,13 +3181,13 @@
         <v>32</v>
       </c>
       <c r="B147" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -3188,13 +3195,13 @@
         <v>32</v>
       </c>
       <c r="B148" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -3202,13 +3209,13 @@
         <v>32</v>
       </c>
       <c r="B149" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -3216,27 +3223,27 @@
         <v>32</v>
       </c>
       <c r="B150" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>215</v>
+        <v>64</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B151" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3244,13 +3251,13 @@
         <v>33</v>
       </c>
       <c r="B152" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3258,13 +3265,13 @@
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -3272,13 +3279,13 @@
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -3286,13 +3293,13 @@
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -3300,13 +3307,13 @@
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -3314,13 +3321,13 @@
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -3328,13 +3335,13 @@
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -3342,13 +3349,13 @@
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -3356,13 +3363,13 @@
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3370,13 +3377,13 @@
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>214</v>
+        <v>171</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3384,13 +3391,13 @@
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3398,13 +3405,13 @@
         <v>33</v>
       </c>
       <c r="B163" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3412,13 +3419,13 @@
         <v>33</v>
       </c>
       <c r="B164" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3426,13 +3433,13 @@
         <v>33</v>
       </c>
       <c r="B165" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3440,13 +3447,13 @@
         <v>33</v>
       </c>
       <c r="B166" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3454,13 +3461,13 @@
         <v>33</v>
       </c>
       <c r="B167" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -3468,27 +3475,27 @@
         <v>33</v>
       </c>
       <c r="B168" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B169" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -3496,13 +3503,13 @@
         <v>34</v>
       </c>
       <c r="B170" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -3510,13 +3517,13 @@
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -3524,13 +3531,13 @@
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -3538,13 +3545,13 @@
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -3552,13 +3559,13 @@
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -3566,13 +3573,13 @@
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -3580,13 +3587,13 @@
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -3594,13 +3601,13 @@
         <v>34</v>
       </c>
       <c r="B177" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -3608,13 +3615,13 @@
         <v>34</v>
       </c>
       <c r="B178" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -3622,13 +3629,13 @@
         <v>34</v>
       </c>
       <c r="B179" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -3636,13 +3643,13 @@
         <v>34</v>
       </c>
       <c r="B180" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -3650,13 +3657,13 @@
         <v>34</v>
       </c>
       <c r="B181" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -3664,13 +3671,13 @@
         <v>34</v>
       </c>
       <c r="B182" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -3678,27 +3685,27 @@
         <v>34</v>
       </c>
       <c r="B183" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>216</v>
+        <v>42</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B184" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -3706,13 +3713,13 @@
         <v>36</v>
       </c>
       <c r="B185" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -3720,13 +3727,13 @@
         <v>36</v>
       </c>
       <c r="B186" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
@@ -3734,13 +3741,13 @@
         <v>36</v>
       </c>
       <c r="B187" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -3748,27 +3755,27 @@
         <v>36</v>
       </c>
       <c r="B188" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B189" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -3776,13 +3783,13 @@
         <v>37</v>
       </c>
       <c r="B190" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -3790,13 +3797,13 @@
         <v>37</v>
       </c>
       <c r="B191" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -3804,13 +3811,13 @@
         <v>37</v>
       </c>
       <c r="B192" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -3818,27 +3825,27 @@
         <v>37</v>
       </c>
       <c r="B193" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B194" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -3846,13 +3853,13 @@
         <v>38</v>
       </c>
       <c r="B195" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -3860,13 +3867,13 @@
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -3874,13 +3881,13 @@
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -3888,13 +3895,13 @@
         <v>38</v>
       </c>
       <c r="B198" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -3902,13 +3909,13 @@
         <v>38</v>
       </c>
       <c r="B199" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -3916,13 +3923,13 @@
         <v>38</v>
       </c>
       <c r="B200" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -3930,13 +3937,13 @@
         <v>38</v>
       </c>
       <c r="B201" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -3944,13 +3951,13 @@
         <v>38</v>
       </c>
       <c r="B202" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -3958,13 +3965,13 @@
         <v>38</v>
       </c>
       <c r="B203" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -3972,33 +3979,47 @@
         <v>38</v>
       </c>
       <c r="B204" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
+        <v>38</v>
+      </c>
+      <c r="B205" s="1">
+        <v>10</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
         <v>39</v>
       </c>
-      <c r="B205" s="1">
+      <c r="B206" s="1">
         <v>0</v>
       </c>
-      <c r="C205" s="2" t="s">
+      <c r="C206" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D205" s="2" t="s">
-        <v>198</v>
+      <c r="D206" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D205">
-    <sortCondition ref="A3:A205"/>
-    <sortCondition ref="B3:B205"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D206">
+    <sortCondition ref="A3:A206"/>
+    <sortCondition ref="B3:B206"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed new member duplicate entry bug, added seasonal member feature
</commit_message>
<xml_diff>
--- a/config/NMRA_Region_Division_Map.xlsx
+++ b/config/NMRA_Region_Division_Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31FB1C9-AB21-5740-A24C-5CCD539F27E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DED88F6-CD48-EA41-9B09-F7788081B517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37820" yWindow="15760" windowWidth="38980" windowHeight="27440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="222">
   <si>
     <t>division</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>Southern Arkansas Area</t>
+  </si>
+  <si>
+    <t>Lakeshores-NY</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1512,16 +1515,16 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1529,10 +1532,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>204</v>
@@ -1543,10 +1546,10 @@
         <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>204</v>
@@ -1557,10 +1560,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>204</v>
@@ -1571,10 +1574,10 @@
         <v>23</v>
       </c>
       <c r="B32" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>204</v>
@@ -1585,10 +1588,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>204</v>
@@ -1599,10 +1602,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>204</v>
@@ -1613,10 +1616,10 @@
         <v>23</v>
       </c>
       <c r="B35" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>216</v>
+        <v>126</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>204</v>
@@ -1627,10 +1630,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>204</v>
@@ -1641,10 +1644,10 @@
         <v>23</v>
       </c>
       <c r="B37" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>204</v>
@@ -1655,10 +1658,10 @@
         <v>23</v>
       </c>
       <c r="B38" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>204</v>
@@ -1666,16 +1669,16 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1683,10 +1686,10 @@
         <v>24</v>
       </c>
       <c r="B40" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>212</v>
@@ -1697,10 +1700,10 @@
         <v>24</v>
       </c>
       <c r="B41" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>212</v>
@@ -1711,10 +1714,10 @@
         <v>24</v>
       </c>
       <c r="B42" s="1">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>212</v>
@@ -1725,10 +1728,10 @@
         <v>24</v>
       </c>
       <c r="B43" s="1">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>212</v>
@@ -1739,10 +1742,10 @@
         <v>24</v>
       </c>
       <c r="B44" s="1">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>212</v>
@@ -1753,10 +1756,10 @@
         <v>24</v>
       </c>
       <c r="B45" s="1">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>212</v>
@@ -1767,10 +1770,10 @@
         <v>24</v>
       </c>
       <c r="B46" s="1">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>212</v>
@@ -1781,10 +1784,10 @@
         <v>24</v>
       </c>
       <c r="B47" s="1">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>212</v>
@@ -1792,16 +1795,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="1">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1809,10 +1812,10 @@
         <v>25</v>
       </c>
       <c r="B49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>207</v>
@@ -1823,10 +1826,10 @@
         <v>25</v>
       </c>
       <c r="B50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>207</v>
@@ -1837,10 +1840,10 @@
         <v>25</v>
       </c>
       <c r="B51" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>207</v>
@@ -1851,10 +1854,10 @@
         <v>25</v>
       </c>
       <c r="B52" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>207</v>
@@ -1865,10 +1868,10 @@
         <v>25</v>
       </c>
       <c r="B53" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>207</v>
@@ -1879,10 +1882,10 @@
         <v>25</v>
       </c>
       <c r="B54" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>207</v>
@@ -1893,10 +1896,10 @@
         <v>25</v>
       </c>
       <c r="B55" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>207</v>
@@ -1904,16 +1907,16 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1921,10 +1924,10 @@
         <v>26</v>
       </c>
       <c r="B57" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>206</v>
@@ -1935,10 +1938,10 @@
         <v>26</v>
       </c>
       <c r="B58" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>206</v>
@@ -1949,10 +1952,10 @@
         <v>26</v>
       </c>
       <c r="B59" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>206</v>
@@ -1963,10 +1966,10 @@
         <v>26</v>
       </c>
       <c r="B60" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>206</v>
@@ -1977,10 +1980,10 @@
         <v>26</v>
       </c>
       <c r="B61" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>206</v>
@@ -1988,16 +1991,16 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B62" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2005,10 +2008,10 @@
         <v>27</v>
       </c>
       <c r="B63" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>209</v>
@@ -2019,10 +2022,10 @@
         <v>27</v>
       </c>
       <c r="B64" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>209</v>
@@ -2033,10 +2036,10 @@
         <v>27</v>
       </c>
       <c r="B65" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>209</v>
@@ -2047,10 +2050,10 @@
         <v>27</v>
       </c>
       <c r="B66" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>209</v>
@@ -2061,10 +2064,10 @@
         <v>27</v>
       </c>
       <c r="B67" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>209</v>
@@ -2075,10 +2078,10 @@
         <v>27</v>
       </c>
       <c r="B68" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>209</v>
@@ -2089,10 +2092,10 @@
         <v>27</v>
       </c>
       <c r="B69" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>209</v>
@@ -2103,10 +2106,10 @@
         <v>27</v>
       </c>
       <c r="B70" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>209</v>
@@ -2117,10 +2120,10 @@
         <v>27</v>
       </c>
       <c r="B71" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>209</v>
@@ -2131,10 +2134,10 @@
         <v>27</v>
       </c>
       <c r="B72" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>209</v>
@@ -2145,10 +2148,10 @@
         <v>27</v>
       </c>
       <c r="B73" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>209</v>
@@ -2159,10 +2162,10 @@
         <v>27</v>
       </c>
       <c r="B74" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>209</v>
@@ -2173,10 +2176,10 @@
         <v>27</v>
       </c>
       <c r="B75" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>209</v>
@@ -2187,10 +2190,10 @@
         <v>27</v>
       </c>
       <c r="B76" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>209</v>
@@ -2201,10 +2204,10 @@
         <v>27</v>
       </c>
       <c r="B77" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>209</v>
@@ -2215,10 +2218,10 @@
         <v>27</v>
       </c>
       <c r="B78" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>209</v>
@@ -2229,10 +2232,10 @@
         <v>27</v>
       </c>
       <c r="B79" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>209</v>
@@ -2240,16 +2243,16 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B80" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2257,10 +2260,10 @@
         <v>28</v>
       </c>
       <c r="B81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>202</v>
@@ -2271,10 +2274,10 @@
         <v>28</v>
       </c>
       <c r="B82" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>202</v>
@@ -2285,10 +2288,10 @@
         <v>28</v>
       </c>
       <c r="B83" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>202</v>
@@ -2299,10 +2302,10 @@
         <v>28</v>
       </c>
       <c r="B84" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>202</v>
@@ -2313,10 +2316,10 @@
         <v>28</v>
       </c>
       <c r="B85" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>202</v>
@@ -2327,10 +2330,10 @@
         <v>28</v>
       </c>
       <c r="B86" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>202</v>
@@ -2341,10 +2344,10 @@
         <v>28</v>
       </c>
       <c r="B87" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>202</v>
@@ -2355,10 +2358,10 @@
         <v>28</v>
       </c>
       <c r="B88" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>202</v>
@@ -2369,10 +2372,10 @@
         <v>28</v>
       </c>
       <c r="B89" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>202</v>
@@ -2383,10 +2386,10 @@
         <v>28</v>
       </c>
       <c r="B90" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>202</v>
@@ -2394,16 +2397,16 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B91" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2411,10 +2414,10 @@
         <v>29</v>
       </c>
       <c r="B92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>200</v>
@@ -2425,10 +2428,10 @@
         <v>29</v>
       </c>
       <c r="B93" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>200</v>
@@ -2439,10 +2442,10 @@
         <v>29</v>
       </c>
       <c r="B94" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>200</v>
@@ -2453,10 +2456,10 @@
         <v>29</v>
       </c>
       <c r="B95" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>200</v>
@@ -2467,10 +2470,10 @@
         <v>29</v>
       </c>
       <c r="B96" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>200</v>
@@ -2481,10 +2484,10 @@
         <v>29</v>
       </c>
       <c r="B97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>200</v>
@@ -2495,10 +2498,10 @@
         <v>29</v>
       </c>
       <c r="B98" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>200</v>
@@ -2509,10 +2512,10 @@
         <v>29</v>
       </c>
       <c r="B99" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>200</v>
@@ -2523,10 +2526,10 @@
         <v>29</v>
       </c>
       <c r="B100" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>200</v>
@@ -2537,10 +2540,10 @@
         <v>29</v>
       </c>
       <c r="B101" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>200</v>
@@ -2551,10 +2554,10 @@
         <v>29</v>
       </c>
       <c r="B102" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>200</v>
@@ -2565,10 +2568,10 @@
         <v>29</v>
       </c>
       <c r="B103" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>200</v>
@@ -2579,10 +2582,10 @@
         <v>29</v>
       </c>
       <c r="B104" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>200</v>
@@ -2593,10 +2596,10 @@
         <v>29</v>
       </c>
       <c r="B105" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>200</v>
@@ -2607,10 +2610,10 @@
         <v>29</v>
       </c>
       <c r="B106" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>200</v>
@@ -2621,10 +2624,10 @@
         <v>29</v>
       </c>
       <c r="B107" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>200</v>
@@ -2635,10 +2638,10 @@
         <v>29</v>
       </c>
       <c r="B108" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>200</v>
@@ -2649,10 +2652,10 @@
         <v>29</v>
       </c>
       <c r="B109" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>200</v>
@@ -2663,10 +2666,10 @@
         <v>29</v>
       </c>
       <c r="B110" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>200</v>
@@ -2677,10 +2680,10 @@
         <v>29</v>
       </c>
       <c r="B111" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>200</v>
@@ -2691,10 +2694,10 @@
         <v>29</v>
       </c>
       <c r="B112" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>200</v>
@@ -2705,10 +2708,10 @@
         <v>29</v>
       </c>
       <c r="B113" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>200</v>
@@ -2719,10 +2722,10 @@
         <v>29</v>
       </c>
       <c r="B114" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>200</v>
@@ -2733,10 +2736,10 @@
         <v>29</v>
       </c>
       <c r="B115" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>220</v>
+        <v>87</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>200</v>
@@ -2744,16 +2747,16 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>88</v>
+        <v>220</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2761,10 +2764,10 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>201</v>
@@ -2775,10 +2778,10 @@
         <v>30</v>
       </c>
       <c r="B118" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>201</v>
@@ -2789,10 +2792,10 @@
         <v>30</v>
       </c>
       <c r="B119" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>201</v>
@@ -2803,10 +2806,10 @@
         <v>30</v>
       </c>
       <c r="B120" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>201</v>
@@ -2817,10 +2820,10 @@
         <v>30</v>
       </c>
       <c r="B121" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>201</v>
@@ -2831,10 +2834,10 @@
         <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>201</v>
@@ -2845,10 +2848,10 @@
         <v>30</v>
       </c>
       <c r="B123" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>201</v>
@@ -2859,10 +2862,10 @@
         <v>30</v>
       </c>
       <c r="B124" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>201</v>
@@ -2873,10 +2876,10 @@
         <v>30</v>
       </c>
       <c r="B125" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>201</v>
@@ -2887,10 +2890,10 @@
         <v>30</v>
       </c>
       <c r="B126" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>201</v>
@@ -2901,10 +2904,10 @@
         <v>30</v>
       </c>
       <c r="B127" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>201</v>
@@ -2915,10 +2918,10 @@
         <v>30</v>
       </c>
       <c r="B128" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>201</v>
@@ -2929,10 +2932,10 @@
         <v>30</v>
       </c>
       <c r="B129" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>201</v>
@@ -2940,16 +2943,16 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B130" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -2957,10 +2960,10 @@
         <v>31</v>
       </c>
       <c r="B131" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>198</v>
@@ -2971,10 +2974,10 @@
         <v>31</v>
       </c>
       <c r="B132" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>198</v>
@@ -2985,10 +2988,10 @@
         <v>31</v>
       </c>
       <c r="B133" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>198</v>
@@ -2999,10 +3002,10 @@
         <v>31</v>
       </c>
       <c r="B134" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>198</v>
@@ -3013,10 +3016,10 @@
         <v>31</v>
       </c>
       <c r="B135" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>198</v>
@@ -3027,10 +3030,10 @@
         <v>31</v>
       </c>
       <c r="B136" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>198</v>
@@ -3041,10 +3044,10 @@
         <v>31</v>
       </c>
       <c r="B137" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>198</v>
@@ -3055,10 +3058,10 @@
         <v>31</v>
       </c>
       <c r="B138" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>198</v>
@@ -3066,16 +3069,16 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B139" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -3083,10 +3086,10 @@
         <v>32</v>
       </c>
       <c r="B140" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>199</v>
@@ -3097,10 +3100,10 @@
         <v>32</v>
       </c>
       <c r="B141" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>199</v>
@@ -3111,10 +3114,10 @@
         <v>32</v>
       </c>
       <c r="B142" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>199</v>
@@ -3125,10 +3128,10 @@
         <v>32</v>
       </c>
       <c r="B143" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>199</v>
@@ -3139,10 +3142,10 @@
         <v>32</v>
       </c>
       <c r="B144" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>199</v>
@@ -3153,10 +3156,10 @@
         <v>32</v>
       </c>
       <c r="B145" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>199</v>
@@ -3167,10 +3170,10 @@
         <v>32</v>
       </c>
       <c r="B146" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>199</v>
@@ -3181,10 +3184,10 @@
         <v>32</v>
       </c>
       <c r="B147" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>199</v>
@@ -3195,10 +3198,10 @@
         <v>32</v>
       </c>
       <c r="B148" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>199</v>
@@ -3209,10 +3212,10 @@
         <v>32</v>
       </c>
       <c r="B149" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>199</v>
@@ -3223,10 +3226,10 @@
         <v>32</v>
       </c>
       <c r="B150" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>199</v>
@@ -3237,10 +3240,10 @@
         <v>32</v>
       </c>
       <c r="B151" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>214</v>
+        <v>64</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>199</v>
@@ -3248,16 +3251,16 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B152" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3265,10 +3268,10 @@
         <v>33</v>
       </c>
       <c r="B153" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>210</v>
@@ -3279,10 +3282,10 @@
         <v>33</v>
       </c>
       <c r="B154" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>210</v>
@@ -3293,10 +3296,10 @@
         <v>33</v>
       </c>
       <c r="B155" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>210</v>
@@ -3307,10 +3310,10 @@
         <v>33</v>
       </c>
       <c r="B156" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>210</v>
@@ -3321,10 +3324,10 @@
         <v>33</v>
       </c>
       <c r="B157" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>210</v>
@@ -3335,10 +3338,10 @@
         <v>33</v>
       </c>
       <c r="B158" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>175</v>
+        <v>95</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>210</v>
@@ -3349,10 +3352,10 @@
         <v>33</v>
       </c>
       <c r="B159" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>210</v>
@@ -3363,10 +3366,10 @@
         <v>33</v>
       </c>
       <c r="B160" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>210</v>
@@ -3377,10 +3380,10 @@
         <v>33</v>
       </c>
       <c r="B161" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>210</v>
@@ -3391,10 +3394,10 @@
         <v>33</v>
       </c>
       <c r="B162" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>210</v>
@@ -3405,10 +3408,10 @@
         <v>33</v>
       </c>
       <c r="B163" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>210</v>
@@ -3419,10 +3422,10 @@
         <v>33</v>
       </c>
       <c r="B164" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>210</v>
@@ -3433,10 +3436,10 @@
         <v>33</v>
       </c>
       <c r="B165" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>210</v>
@@ -3447,10 +3450,10 @@
         <v>33</v>
       </c>
       <c r="B166" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>210</v>
@@ -3461,10 +3464,10 @@
         <v>33</v>
       </c>
       <c r="B167" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>210</v>
@@ -3475,10 +3478,10 @@
         <v>33</v>
       </c>
       <c r="B168" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>210</v>
@@ -3489,10 +3492,10 @@
         <v>33</v>
       </c>
       <c r="B169" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>210</v>
@@ -3500,16 +3503,16 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B170" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -3517,10 +3520,10 @@
         <v>34</v>
       </c>
       <c r="B171" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>196</v>
@@ -3531,10 +3534,10 @@
         <v>34</v>
       </c>
       <c r="B172" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>196</v>
@@ -3545,10 +3548,10 @@
         <v>34</v>
       </c>
       <c r="B173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>196</v>
@@ -3559,10 +3562,10 @@
         <v>34</v>
       </c>
       <c r="B174" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>196</v>
@@ -3573,10 +3576,10 @@
         <v>34</v>
       </c>
       <c r="B175" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>196</v>
@@ -3587,10 +3590,10 @@
         <v>34</v>
       </c>
       <c r="B176" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>196</v>
@@ -3601,10 +3604,10 @@
         <v>34</v>
       </c>
       <c r="B177" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>196</v>
@@ -3615,10 +3618,10 @@
         <v>34</v>
       </c>
       <c r="B178" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>196</v>
@@ -3629,10 +3632,10 @@
         <v>34</v>
       </c>
       <c r="B179" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>196</v>
@@ -3643,10 +3646,10 @@
         <v>34</v>
       </c>
       <c r="B180" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>196</v>
@@ -3657,10 +3660,10 @@
         <v>34</v>
       </c>
       <c r="B181" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>196</v>
@@ -3671,10 +3674,10 @@
         <v>34</v>
       </c>
       <c r="B182" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>196</v>
@@ -3685,10 +3688,10 @@
         <v>34</v>
       </c>
       <c r="B183" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>196</v>
@@ -3699,10 +3702,10 @@
         <v>34</v>
       </c>
       <c r="B184" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>215</v>
+        <v>42</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>196</v>
@@ -3710,16 +3713,16 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B185" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -3727,10 +3730,10 @@
         <v>36</v>
       </c>
       <c r="B186" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>211</v>
@@ -3741,10 +3744,10 @@
         <v>36</v>
       </c>
       <c r="B187" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>211</v>
@@ -3755,10 +3758,10 @@
         <v>36</v>
       </c>
       <c r="B188" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>211</v>
@@ -3769,10 +3772,10 @@
         <v>36</v>
       </c>
       <c r="B189" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>211</v>
@@ -3780,16 +3783,16 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B190" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -3797,10 +3800,10 @@
         <v>37</v>
       </c>
       <c r="B191" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>208</v>
@@ -3811,10 +3814,10 @@
         <v>37</v>
       </c>
       <c r="B192" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>208</v>
@@ -3825,10 +3828,10 @@
         <v>37</v>
       </c>
       <c r="B193" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>208</v>
@@ -3839,10 +3842,10 @@
         <v>37</v>
       </c>
       <c r="B194" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>208</v>
@@ -3850,16 +3853,16 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B195" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -3867,10 +3870,10 @@
         <v>38</v>
       </c>
       <c r="B196" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>195</v>
@@ -3881,10 +3884,10 @@
         <v>38</v>
       </c>
       <c r="B197" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>195</v>
@@ -3895,10 +3898,10 @@
         <v>38</v>
       </c>
       <c r="B198" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>195</v>
@@ -3909,10 +3912,10 @@
         <v>38</v>
       </c>
       <c r="B199" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>195</v>
@@ -3923,10 +3926,10 @@
         <v>38</v>
       </c>
       <c r="B200" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>195</v>
@@ -3937,10 +3940,10 @@
         <v>38</v>
       </c>
       <c r="B201" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>195</v>
@@ -3951,10 +3954,10 @@
         <v>38</v>
       </c>
       <c r="B202" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>195</v>
@@ -3965,10 +3968,10 @@
         <v>38</v>
       </c>
       <c r="B203" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>195</v>
@@ -3979,10 +3982,10 @@
         <v>38</v>
       </c>
       <c r="B204" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>195</v>
@@ -3993,10 +3996,10 @@
         <v>38</v>
       </c>
       <c r="B205" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>195</v>
@@ -4004,22 +4007,36 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
+        <v>38</v>
+      </c>
+      <c r="B206" s="1">
+        <v>10</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
         <v>39</v>
       </c>
-      <c r="B206" s="1">
+      <c r="B207" s="1">
         <v>0</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="C207" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D206" s="2" t="s">
+      <c r="D207" s="2" t="s">
         <v>197</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D206">
-    <sortCondition ref="A3:A206"/>
-    <sortCondition ref="B3:B206"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D207">
+    <sortCondition ref="A3:A207"/>
+    <sortCondition ref="B3:B207"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>